<commit_message>
add more documentation and implement report_TADs
</commit_message>
<xml_diff>
--- a/example_results/genes_by_loci_all.xlsx
+++ b/example_results/genes_by_loci_all.xlsx
@@ -110,13 +110,13 @@
     <t>CD74; TNIP1; RPS14; ATOX1</t>
   </si>
   <si>
-    <t>PPP2R3C (hacat_stim_2,hacat_stim only), TAD level:2; KIAA0391 (hacat_stim_2,hacat_stim only), TAD level:2; PSMA6 (hacat_stim_2,hacat_stim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>CS (all), TAD level:3; BAZ2A (hacat_stim_2 only), TAD level:2; IL23A (hacat_stim_2,hacat_stim only), TAD level:3; TIMELESS (hacat_stim_2,hacat_stim only), TAD level:2; GDF11 (hacat_stim_2,hacat_stim only), TAD level:outside tad; GLS2 (hacat_stim_2,hacat_stim only), TAD level:2; COQ10A (all), TAD level:3; PAN2 (all), TAD level:3; ZC3H10 (hacat_stim_2,hacat_stim only), TAD level:not found; NABP2 (hacat_stim_2 only), TAD level:3; SMARCC2 (hacat_stim_2,hacat_stim only), TAD level:3; ESYT1 (all), TAD level:not found; ANKRD52 (hacat_stim only), TAD level:3; STAT2 (all), TAD level:3; SPRYD4 (all), TAD level:2; RNF41 (hacat_stim_2 only), TAD level:3; RPL41 (hacat_stim_2,hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>REV3L (hacat_stim_2,hacat_stim only), TAD level:1; TRAF3IP2 (hacat_stim_2,hacat_stim only), TAD level:3; MFSD4B (all), TAD level:1</t>
+    <t>PPP2R3C (hacat_stim_2, hacat_stim only), TAD level:2; KIAA0391 (hacat_stim_2, hacat_stim only), TAD level:2; PSMA6 (hacat_stim_2, hacat_stim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>CS (all), TAD level:3; BAZ2A (hacat_stim_2 only), TAD level:2; IL23A (hacat_stim_2, hacat_stim only), TAD level:3; TIMELESS (hacat_stim_2, hacat_stim only), TAD level:2; GDF11 (hacat_stim_2, hacat_stim only), TAD level:outside tad; GLS2 (hacat_stim_2, hacat_stim only), TAD level:2; COQ10A (all), TAD level:3; PAN2 (all), TAD level:3; ZC3H10 (hacat_stim_2, hacat_stim only), TAD level:not found; NABP2 (hacat_stim_2 only), TAD level:3; SMARCC2 (hacat_stim_2, hacat_stim only), TAD level:3; ESYT1 (all), TAD level:not found; ANKRD52 (hacat_stim only), TAD level:3; STAT2 (all), TAD level:3; SPRYD4 (all), TAD level:2; RNF41 (hacat_stim_2 only), TAD level:3; RPL41 (hacat_stim_2, hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>REV3L (hacat_stim_2, hacat_stim only), TAD level:1; TRAF3IP2 (hacat_stim_2, hacat_stim only), TAD level:3; MFSD4B (all), TAD level:1</t>
   </si>
   <si>
     <t>TTC1 (hacat_stim only), TAD level:1</t>
@@ -125,19 +125,19 @@
     <t>P4HA2 (hacat_stim only), TAD level:2; RAPGEF6 (hacat_stim only), TAD level:not found; SLC22A4 (hacat_stim only), TAD level:2; SLC22A5 (hacat_stim_2 only), TAD level:2</t>
   </si>
   <si>
-    <t>STPG1 (all), TAD level:4; NIPAL3 (all), TAD level:4; SRRM1 (hacat_stim_2,hacat_stim only), TAD level:2; IL22RA1 (hacat_stim_2 only), TAD level:3; GRHL3 (hacat_stim only), TAD level:4; CLIC4 (hacat_stim only), TAD level:1; IFNLR1 (all), TAD level:3</t>
-  </si>
-  <si>
-    <t>NDST1 (hacat_stim only), TAD level:1; TNIP1 (hacat_stim_2,hacat_stim only), TAD level:2; ATOX1 (hacat_stim_2 only), TAD level:not found; GM2A (hacat_stim_2 only), TAD level:2</t>
-  </si>
-  <si>
-    <t>PPP2R3C (hacat_unstim_2,hacat_unstim only), TAD level:2; KIAA0391 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>CS (all), TAD level:3; TIMELESS (hacat_unstim_2,hacat_unstim only), TAD level:2; GDF11 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; COQ10A (all), TAD level:3; PAN2 (all), TAD level:3; ZC3H10 (hacat_unstim_2,hacat_unstim only), TAD level:not found; SMARCC2 (hacat_unstim_2,hacat_unstim only), TAD level:3; ESYT1 (hacat_unstim_2,hacat_unstim only), TAD level:not found; STAT6 (hacat_unstim only), TAD level:2; STAT2 (all), TAD level:3; SPRYD4 (all), TAD level:2; RPL41 (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>REV3L (hacat_unstim_2,hacat_unstim only), TAD level:1; TRAF3IP2 (hacat_unstim_2,hacat_unstim only), TAD level:3; MFSD4B (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
+    <t>STPG1 (all), TAD level:4; NIPAL3 (all), TAD level:4; SRRM1 (hacat_stim_2, hacat_stim only), TAD level:2; IL22RA1 (hacat_stim_2 only), TAD level:3; GRHL3 (hacat_stim only), TAD level:4; CLIC4 (hacat_stim only), TAD level:1; IFNLR1 (all), TAD level:3</t>
+  </si>
+  <si>
+    <t>NDST1 (hacat_stim only), TAD level:1; TNIP1 (hacat_stim_2, hacat_stim only), TAD level:2; ATOX1 (hacat_stim_2 only), TAD level:not found; GM2A (hacat_stim_2 only), TAD level:2</t>
+  </si>
+  <si>
+    <t>PPP2R3C (hacat_unstim_2, hacat_unstim only), TAD level:2; KIAA0391 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>CS (all), TAD level:3; TIMELESS (hacat_unstim_2, hacat_unstim only), TAD level:2; GDF11 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; COQ10A (all), TAD level:3; PAN2 (all), TAD level:3; ZC3H10 (hacat_unstim_2, hacat_unstim only), TAD level:not found; SMARCC2 (hacat_unstim_2, hacat_unstim only), TAD level:3; ESYT1 (hacat_unstim_2, hacat_unstim only), TAD level:not found; STAT6 (hacat_unstim only), TAD level:2; STAT2 (all), TAD level:3; SPRYD4 (all), TAD level:2; RPL41 (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>REV3L (hacat_unstim_2, hacat_unstim only), TAD level:1; TRAF3IP2 (hacat_unstim_2, hacat_unstim only), TAD level:3; MFSD4B (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
   </si>
   <si>
     <t>TTC1 (hacat_unstim only), TAD level:1</t>
@@ -146,16 +146,16 @@
     <t>IRF1 (hacat_unstim only), TAD level:1; PDLIM4 (hacat_unstim only), TAD level:1; RAPGEF6 (hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
-    <t>STPG1 (all), TAD level:3; NIPAL3 (all), TAD level:3; SRRM1 (hacat_unstim_2,hacat_unstim only), TAD level:2; GRHL3 (all), TAD level:3; IFNLR1 (all), TAD level:3</t>
-  </si>
-  <si>
-    <t>TNIP1 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>CS (all), TAD level:1; IL23A (myla only), TAD level:1; TIMELESS (all), TAD level:1; CD63 (myla_2 only), TAD level:1; GDF11 (myla_1,myla only), TAD level:1; COQ10A (all), TAD level:1; PAN2 (all), TAD level:1; SMARCC2 (myla_2,myla only), TAD level:1; ESYT1 (all), TAD level:1; STAT2 (all), TAD level:1; SPRYD4 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>ICAM1 (myla_1,myla only), TAD level:1; TYK2 (myla_1,myla only), TAD level:not found</t>
+    <t>STPG1 (all), TAD level:3; NIPAL3 (all), TAD level:3; SRRM1 (hacat_unstim_2, hacat_unstim only), TAD level:2; GRHL3 (all), TAD level:3; IFNLR1 (all), TAD level:3</t>
+  </si>
+  <si>
+    <t>TNIP1 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>CS (all), TAD level:1; IL23A (myla only), TAD level:1; TIMELESS (all), TAD level:1; CD63 (myla_2 only), TAD level:1; GDF11 (myla_1, myla only), TAD level:1; COQ10A (all), TAD level:1; PAN2 (all), TAD level:1; SMARCC2 (myla_2, myla only), TAD level:1; ESYT1 (all), TAD level:1; STAT2 (all), TAD level:1; SPRYD4 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>ICAM1 (myla_1, myla only), TAD level:1; TYK2 (myla_1, myla only), TAD level:not found</t>
   </si>
   <si>
     <t>IRF1 (all), TAD level:1; SLC22A5 (myla only), TAD level:2</t>
@@ -164,16 +164,16 @@
     <t>STPG1 (all), TAD level:3; NIPAL3 (all), TAD level:3; RCAN3 (myla only), TAD level:3; SRRM1 (all), TAD level:2</t>
   </si>
   <si>
-    <t>CD74 (myla_1,myla only), TAD level:outside tad; RBM22 (myla only), TAD level:2; DCTN4 (myla_2 only), TAD level:2; TNIP1 (all), TAD level:2; G3BP1 (myla only), TAD level:not found; RPS14 (myla_1,myla only), TAD level:not found; ATOX1 (myla_1,myla only), TAD level:not found; GM2A (myla_2,myla only), TAD level:3</t>
+    <t>CD74 (myla_1, myla only), TAD level:outside tad; RBM22 (myla only), TAD level:2; DCTN4 (myla_2 only), TAD level:2; TNIP1 (all), TAD level:2; G3BP1 (myla only), TAD level:not found; RPS14 (myla_1, myla only), TAD level:not found; ATOX1 (myla_1, myla only), TAD level:not found; GM2A (myla_2, myla only), TAD level:3</t>
   </si>
   <si>
     <t>SLC35D1 (all); GADD45A (naive_T_2 only); PDE4B (all); MIER1 (all)</t>
   </si>
   <si>
-    <t>CS (all); ERBB3 (all); BAZ2A (all); IL23A (all); ATP5F1B (all); PTGES3 (naive_T_1,naive_T only); RAB5B (all); TIMELESS (all); ARHGAP9 (all); NCKAP1L (naive_T only); ORMDL2 (all); DNAJC14 (all); GDF11 (all); GLS2 (naive_T_1,naive_T only); RDH5 (all); BLOC1S1 (all); CDK4 (naive_T_1,naive_T only); TSPAN31 (naive_T_1,naive_T only); COQ10A (all); PAN2 (all); ZC3H10 (all); OS9 (naive_T_1,naive_T only); MARCH9 (naive_T_1,naive_T only); SUOX (naive_T only); SMARCC2 (all); ESYT1 (all); STAT6 (naive_T only); MARS (all); MBD6 (naive_T_1,naive_T only); PA2G4 (all); STAT2 (all); DDIT3 (naive_T_1,naive_T only); SPRYD4 (all); PMEL (all); NACA (naive_T_1,naive_T only); RPS26 (all); SARNP (all); RPL41 (all); BLOC1S1-RDH5 (all)</t>
-  </si>
-  <si>
-    <t>TTC1 (naive_T_1,naive_T only)</t>
+    <t>CS (all); ERBB3 (all); BAZ2A (all); IL23A (all); ATP5F1B (all); PTGES3 (naive_T_1, naive_T only); RAB5B (all); TIMELESS (all); ARHGAP9 (all); NCKAP1L (naive_T only); ORMDL2 (all); DNAJC14 (all); GDF11 (all); GLS2 (naive_T_1, naive_T only); RDH5 (all); BLOC1S1 (all); CDK4 (naive_T_1, naive_T only); TSPAN31 (naive_T_1, naive_T only); COQ10A (all); PAN2 (all); ZC3H10 (all); OS9 (naive_T_1, naive_T only); MARCH9 (naive_T_1, naive_T only); SUOX (naive_T only); SMARCC2 (all); ESYT1 (all); STAT6 (naive_T only); MARS (all); MBD6 (naive_T_1, naive_T only); PA2G4 (all); STAT2 (all); DDIT3 (naive_T_1, naive_T only); SPRYD4 (all); PMEL (all); NACA (naive_T_1, naive_T only); RPS26 (all); SARNP (all); RPL41 (all); BLOC1S1-RDH5 (all)</t>
+  </si>
+  <si>
+    <t>TTC1 (naive_T_1, naive_T only)</t>
   </si>
   <si>
     <t>FNIP1 (naive_T only)</t>
@@ -182,7 +182,7 @@
     <t>STPG1 (all); NIPAL3 (naive_T only); SRRM1 (all); IFNLR1 (all)</t>
   </si>
   <si>
-    <t>CD74 (all); DCTN4 (naive_T_1,naive_T only); TNIP1 (all); RPS14 (all); GM2A (naive_T only)</t>
+    <t>CD74 (all); DCTN4 (naive_T_1, naive_T only); TNIP1 (all); RPS14 (all); GM2A (naive_T only)</t>
   </si>
   <si>
     <t>rs1148732</t>
@@ -392,22 +392,22 @@
     <t>APOLD1 (hacat_stim_1 only), TAD level:not found</t>
   </si>
   <si>
-    <t>CDKN2B (hacat_stim_2,hacat_stim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>SEC62 (hacat_stim_2,hacat_stim only), TAD level:3; MYNN (all), TAD level:1; MECOM (all), TAD level:2; ACTRT3 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>PICK1 (hacat_stim_2,hacat_stim only), TAD level:1; DMC1 (hacat_stim_2,hacat_stim only), TAD level:1; TOMM22 (hacat_stim only), TAD level:not found; BAIAP2L2 (hacat_stim_2,hacat_stim only), TAD level:1; PLA2G6 (all), TAD level:1; MAFF (all), TAD level:1; TMEM184B (hacat_stim_2,hacat_stim only), TAD level:1; CSNK1E (hacat_stim_2,hacat_stim only), TAD level:1</t>
+    <t>CDKN2B (hacat_stim_2, hacat_stim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>SEC62 (hacat_stim_2, hacat_stim only), TAD level:3; MYNN (all), TAD level:1; MECOM (all), TAD level:2; ACTRT3 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>PICK1 (hacat_stim_2, hacat_stim only), TAD level:1; DMC1 (hacat_stim_2, hacat_stim only), TAD level:1; TOMM22 (hacat_stim only), TAD level:not found; BAIAP2L2 (hacat_stim_2, hacat_stim only), TAD level:1; PLA2G6 (all), TAD level:1; MAFF (all), TAD level:1; TMEM184B (hacat_stim_2, hacat_stim only), TAD level:1; CSNK1E (hacat_stim_2, hacat_stim only), TAD level:1</t>
   </si>
   <si>
     <t>ZNF462 (hacat_stim_2 only), TAD level:1</t>
   </si>
   <si>
-    <t>HDAC9 (hacat_stim_2,hacat_stim only), TAD level:not found; AHR (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>SOX4 (hacat_stim_2,hacat_stim only), TAD level:1</t>
+    <t>HDAC9 (hacat_stim_2, hacat_stim only), TAD level:not found; AHR (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>SOX4 (hacat_stim_2, hacat_stim only), TAD level:1</t>
   </si>
   <si>
     <t>SYNE2 (all), TAD level:3</t>
@@ -419,52 +419,52 @@
     <t>CLPTM1L (all), TAD level:2</t>
   </si>
   <si>
-    <t>GDI2 (all), TAD level:2; FAM208B (hacat_stim_2,hacat_stim only), TAD level:2; ANKRD16 (hacat_stim_2,hacat_stim only), TAD level:2; NET1 (hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>CYP1B1 (hacat_stim_2,hacat_stim only), TAD level:5</t>
-  </si>
-  <si>
-    <t>CCND1 (hacat_stim_2,hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>EDEM2 (all), TAD level:3; GSS (hacat_stim_2,hacat_stim only), TAD level:3; TRPC4AP (hacat_stim_2,hacat_stim only), TAD level:3; AHCY (hacat_stim only), TAD level:2; PIGU (hacat_stim_2,hacat_stim only), TAD level:3; DYNLRB1 (hacat_stim_2,hacat_stim only), TAD level:3; CEP250 (hacat_stim_2,hacat_stim only), TAD level:2; MMP24OS (hacat_stim_2,hacat_stim only), TAD level:3; EIF6 (hacat_stim_2,hacat_stim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>APH1A (hacat_stim_2,hacat_stim only), TAD level:not found; C1orf54 (hacat_stim_2,hacat_stim only), TAD level:not found; ECM1 (hacat_stim only), TAD level:1; TARS2 (all), TAD level:1; ADAMTSL4 (all), TAD level:1; MCL1 (hacat_stim_2,hacat_stim only), TAD level:1; ANP32E (hacat_stim_2,hacat_stim only), TAD level:not found; CERS2 (all), TAD level:2; ENSA (hacat_stim_2,hacat_stim only), TAD level:2; GOLPH3L (all), TAD level:2; CIART (hacat_stim only), TAD level:1; RPRD2 (hacat_stim_2,hacat_stim only), TAD level:1; CTSS (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>ACAT1 (hacat_stim only), TAD level:not found; EXPH5 (all), TAD level:1; NPAT (all), TAD level:not found; ATM (all), TAD level:1; C11orf65 (all), TAD level:1; DDX10 (all), TAD level:not found; KDELC2 (hacat_stim_2,hacat_stim only), TAD level:1</t>
+    <t>GDI2 (all), TAD level:2; FAM208B (hacat_stim_2, hacat_stim only), TAD level:2; ANKRD16 (hacat_stim_2, hacat_stim only), TAD level:2; NET1 (hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>CYP1B1 (hacat_stim_2, hacat_stim only), TAD level:5</t>
+  </si>
+  <si>
+    <t>CCND1 (hacat_stim_2, hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>EDEM2 (all), TAD level:3; GSS (hacat_stim_2, hacat_stim only), TAD level:3; TRPC4AP (hacat_stim_2, hacat_stim only), TAD level:3; AHCY (hacat_stim only), TAD level:2; PIGU (hacat_stim_2, hacat_stim only), TAD level:3; DYNLRB1 (hacat_stim_2, hacat_stim only), TAD level:3; CEP250 (hacat_stim_2, hacat_stim only), TAD level:2; MMP24OS (hacat_stim_2, hacat_stim only), TAD level:3; EIF6 (hacat_stim_2, hacat_stim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>APH1A (hacat_stim_2, hacat_stim only), TAD level:not found; C1orf54 (hacat_stim_2, hacat_stim only), TAD level:not found; ECM1 (hacat_stim only), TAD level:1; TARS2 (all), TAD level:1; ADAMTSL4 (all), TAD level:1; MCL1 (hacat_stim_2, hacat_stim only), TAD level:1; ANP32E (hacat_stim_2, hacat_stim only), TAD level:not found; CERS2 (all), TAD level:2; ENSA (hacat_stim_2, hacat_stim only), TAD level:2; GOLPH3L (all), TAD level:2; CIART (hacat_stim only), TAD level:1; RPRD2 (hacat_stim_2, hacat_stim only), TAD level:1; CTSS (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>ACAT1 (hacat_stim only), TAD level:not found; EXPH5 (all), TAD level:1; NPAT (all), TAD level:not found; ATM (all), TAD level:1; C11orf65 (all), TAD level:1; DDX10 (all), TAD level:not found; KDELC2 (hacat_stim_2, hacat_stim only), TAD level:1</t>
   </si>
   <si>
     <t>KITLG (all), TAD level:2; DUSP6 (hacat_stim only), TAD level:1; TMTC3 (all), TAD level:2; CEP290 (all), TAD level:not found</t>
   </si>
   <si>
-    <t>DBNDD1 (hacat_stim_2,hacat_stim only), TAD level:not found; VPS9D1 (hacat_stim only), TAD level:not found; PIEZO1 (all), TAD level:outside tad; TCF25 (hacat_stim_2,hacat_stim only), TAD level:not found; GALNS (hacat_stim_2,hacat_stim only), TAD level:outside tad; GAS8 (hacat_stim_2,hacat_stim only), TAD level:not found; SPATA2L (hacat_stim_2,hacat_stim only), TAD level:not found; CDT1 (hacat_stim only), TAD level:outside tad; TRAPPC2L (hacat_stim_2,hacat_stim only), TAD level:outside tad; ANKRD11 (hacat_stim only), TAD level:outside tad; RPL13 (hacat_stim_2,hacat_stim only), TAD level:not found; ZNF778 (hacat_stim_2,hacat_stim only), TAD level:outside tad; CPNE7 (all), TAD level:not found; SPG7 (hacat_stim_2,hacat_stim only), TAD level:outside tad; MC1R (hacat_stim only), TAD level:not found; TUBB3 (hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>ALS2 (hacat_stim_2,hacat_stim only), TAD level:1; CASP8 (all), TAD level:not found; STRADB (hacat_stim_2,hacat_stim only), TAD level:2; TRAK2 (hacat_stim_2,hacat_stim only), TAD level:2; TMEM237 (all), TAD level:2; NIF3L1 (hacat_stim_2 only), TAD level:not found; PPIL3 (hacat_stim_2 only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>MTAP (all), TAD level:2; CDKN2A (hacat_stim_2,hacat_stim only), TAD level:3; KLHL9 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>EMP1 (hacat_unstim_2 only), TAD level:outside tad; APOLD1 (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>SEC62 (hacat_unstim_2,hacat_unstim only), TAD level:3; MYNN (all), TAD level:1; MECOM (hacat_unstim_2,hacat_unstim only), TAD level:2; ACTRT3 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>PICK1 (hacat_unstim only), TAD level:2; DDX17 (hacat_unstim only), TAD level:2; MAFF (all), TAD level:2; TMEM184B (all), TAD level:2; CSNK1E (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>HDAC9 (hacat_unstim only), TAD level:not found; AHR (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>SYNE2 (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>PPARGC1B (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
+    <t>DBNDD1 (hacat_stim_2, hacat_stim only), TAD level:not found; VPS9D1 (hacat_stim only), TAD level:not found; PIEZO1 (all), TAD level:outside tad; TCF25 (hacat_stim_2, hacat_stim only), TAD level:not found; GALNS (hacat_stim_2, hacat_stim only), TAD level:outside tad; GAS8 (hacat_stim_2, hacat_stim only), TAD level:not found; SPATA2L (hacat_stim_2, hacat_stim only), TAD level:not found; CDT1 (hacat_stim only), TAD level:outside tad; TRAPPC2L (hacat_stim_2, hacat_stim only), TAD level:outside tad; ANKRD11 (hacat_stim only), TAD level:outside tad; RPL13 (hacat_stim_2, hacat_stim only), TAD level:not found; ZNF778 (hacat_stim_2, hacat_stim only), TAD level:outside tad; CPNE7 (all), TAD level:not found; SPG7 (hacat_stim_2, hacat_stim only), TAD level:outside tad; MC1R (hacat_stim only), TAD level:not found; TUBB3 (hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>ALS2 (hacat_stim_2, hacat_stim only), TAD level:1; CASP8 (all), TAD level:not found; STRADB (hacat_stim_2, hacat_stim only), TAD level:2; TRAK2 (hacat_stim_2, hacat_stim only), TAD level:2; TMEM237 (all), TAD level:2; NIF3L1 (hacat_stim_2 only), TAD level:not found; PPIL3 (hacat_stim_2 only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>MTAP (all), TAD level:2; CDKN2A (hacat_stim_2, hacat_stim only), TAD level:3; KLHL9 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>EMP1 (hacat_unstim_2 only), TAD level:outside tad; APOLD1 (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>SEC62 (hacat_unstim_2, hacat_unstim only), TAD level:3; MYNN (all), TAD level:1; MECOM (hacat_unstim_2, hacat_unstim only), TAD level:2; ACTRT3 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>PICK1 (hacat_unstim only), TAD level:2; DDX17 (hacat_unstim only), TAD level:2; MAFF (all), TAD level:2; TMEM184B (all), TAD level:2; CSNK1E (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>HDAC9 (hacat_unstim only), TAD level:not found; AHR (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>SYNE2 (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>PPARGC1B (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
   </si>
   <si>
     <t>PARP1 (all), TAD level:1</t>
@@ -473,55 +473,55 @@
     <t>CLPTM1L (all), TAD level:2; LPCAT1 (hacat_unstim only), TAD level:2</t>
   </si>
   <si>
-    <t>GDI2 (all), TAD level:2; ANKRD16 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>RMDN2 (hacat_unstim_2,hacat_unstim only), TAD level:3; CYP1B1 (hacat_unstim_2,hacat_unstim only), TAD level:4</t>
+    <t>GDI2 (all), TAD level:2; ANKRD16 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>RMDN2 (hacat_unstim_2, hacat_unstim only), TAD level:3; CYP1B1 (hacat_unstim_2, hacat_unstim only), TAD level:4</t>
   </si>
   <si>
     <t>CCND1 (hacat_unstim only), TAD level:2</t>
   </si>
   <si>
-    <t>TP53INP2 (hacat_unstim_2,hacat_unstim only), TAD level:4; EDEM2 (hacat_unstim_1,hacat_unstim only), TAD level:3; GSS (hacat_unstim_2,hacat_unstim only), TAD level:3; TRPC4AP (hacat_unstim_2,hacat_unstim only), TAD level:3; AHCY (hacat_unstim only), TAD level:2; PIGU (hacat_unstim_2,hacat_unstim only), TAD level:3; MMP24OS (hacat_unstim only), TAD level:3; EIF6 (hacat_unstim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>APH1A (all), TAD level:1; C1orf54 (all), TAD level:1; ECM1 (hacat_unstim_2,hacat_unstim only), TAD level:3; TARS2 (hacat_unstim_2,hacat_unstim only), TAD level:3; ADAMTSL4 (all), TAD level:3; ANP32E (hacat_unstim_2,hacat_unstim only), TAD level:1; MINDY1 (hacat_unstim_2,hacat_unstim only), TAD level:2; CERS2 (all), TAD level:4; ENSA (hacat_unstim only), TAD level:4; GOLPH3L (all), TAD level:4; CIART (hacat_unstim only), TAD level:1; RPRD2 (hacat_unstim only), TAD level:3; CTSS (all), TAD level:4</t>
-  </si>
-  <si>
-    <t>ACAT1 (hacat_unstim_2,hacat_unstim only), TAD level:1; EXPH5 (all), TAD level:1; NPAT (hacat_unstim_2,hacat_unstim only), TAD level:1; ATM (hacat_unstim_2,hacat_unstim only), TAD level:1; C11orf65 (all), TAD level:1; DDX10 (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
+    <t>TP53INP2 (hacat_unstim_2, hacat_unstim only), TAD level:4; EDEM2 (hacat_unstim_1, hacat_unstim only), TAD level:3; GSS (hacat_unstim_2, hacat_unstim only), TAD level:3; TRPC4AP (hacat_unstim_2, hacat_unstim only), TAD level:3; AHCY (hacat_unstim only), TAD level:2; PIGU (hacat_unstim_2, hacat_unstim only), TAD level:3; MMP24OS (hacat_unstim only), TAD level:3; EIF6 (hacat_unstim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>APH1A (all), TAD level:1; C1orf54 (all), TAD level:1; ECM1 (hacat_unstim_2, hacat_unstim only), TAD level:3; TARS2 (hacat_unstim_2, hacat_unstim only), TAD level:3; ADAMTSL4 (all), TAD level:3; ANP32E (hacat_unstim_2, hacat_unstim only), TAD level:1; MINDY1 (hacat_unstim_2, hacat_unstim only), TAD level:2; CERS2 (all), TAD level:4; ENSA (hacat_unstim only), TAD level:4; GOLPH3L (all), TAD level:4; CIART (hacat_unstim only), TAD level:1; RPRD2 (hacat_unstim only), TAD level:3; CTSS (all), TAD level:4</t>
+  </si>
+  <si>
+    <t>ACAT1 (hacat_unstim_2, hacat_unstim only), TAD level:1; EXPH5 (all), TAD level:1; NPAT (hacat_unstim_2, hacat_unstim only), TAD level:1; ATM (hacat_unstim_2, hacat_unstim only), TAD level:1; C11orf65 (all), TAD level:1; DDX10 (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
     <t>KITLG (all), TAD level:2; POC1B (hacat_unstim only), TAD level:not found; TMTC3 (all), TAD level:2; CEP290 (all), TAD level:not found</t>
   </si>
   <si>
-    <t>DBNDD1 (hacat_unstim_2,hacat_unstim only), TAD level:not found; VPS9D1 (all), TAD level:not found; PIEZO1 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; DEF8 (hacat_unstim_2,hacat_unstim only), TAD level:not found; TCF25 (all), TAD level:not found; GAS8 (hacat_unstim_2,hacat_unstim only), TAD level:not found; ZNF276 (hacat_unstim_1,hacat_unstim only), TAD level:not found; CDT1 (hacat_unstim_1,hacat_unstim only), TAD level:outside tad; ANKRD11 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; RPL13 (hacat_unstim_2,hacat_unstim only), TAD level:not found; ZNF778 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; CPNE7 (all), TAD level:not found; CDK10 (hacat_unstim_2,hacat_unstim only), TAD level:not found; SPG7 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; MC1R (all), TAD level:not found; TUBB3 (all), TAD level:not found</t>
-  </si>
-  <si>
-    <t>ALS2 (hacat_unstim_2,hacat_unstim only), TAD level:1; NOP58 (hacat_unstim_2,hacat_unstim only), TAD level:not found; CASP8 (all), TAD level:not found; STRADB (hacat_unstim_2,hacat_unstim only), TAD level:2; TRAK2 (hacat_unstim_2 only), TAD level:2; TMEM237 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>MTAP (all), TAD level:2; CDKN2A (hacat_unstim_2,hacat_unstim only), TAD level:3; KLHL9 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>APOLD1 (myla_1,myla only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>DUSP22 (myla_1,myla only), TAD level:1; EXOC2 (myla_1,myla only), TAD level:1</t>
-  </si>
-  <si>
-    <t>SEC62 (myla_1,myla only), TAD level:1; MYNN (all), TAD level:not found; SKIL (all), TAD level:1; PRKCI (myla only), TAD level:1; RPL22L1 (all), TAD level:not found; PHC3 (myla_2,myla only), TAD level:1; GPR160 (myla_1 only), TAD level:1; ACTRT3 (all), TAD level:not found</t>
-  </si>
-  <si>
-    <t>CBY1 (myla_1,myla only), TAD level:2; TOMM22 (myla only), TAD level:2; JOSD1 (myla_1,myla only), TAD level:2; PLA2G6 (all), TAD level:2; FAM227A (myla_1,myla only), TAD level:2; CSNK1E (myla only), TAD level:2</t>
+    <t>DBNDD1 (hacat_unstim_2, hacat_unstim only), TAD level:not found; VPS9D1 (all), TAD level:not found; PIEZO1 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; DEF8 (hacat_unstim_2, hacat_unstim only), TAD level:not found; TCF25 (all), TAD level:not found; GAS8 (hacat_unstim_2, hacat_unstim only), TAD level:not found; ZNF276 (hacat_unstim_1, hacat_unstim only), TAD level:not found; CDT1 (hacat_unstim_1, hacat_unstim only), TAD level:outside tad; ANKRD11 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; RPL13 (hacat_unstim_2, hacat_unstim only), TAD level:not found; ZNF778 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; CPNE7 (all), TAD level:not found; CDK10 (hacat_unstim_2, hacat_unstim only), TAD level:not found; SPG7 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; MC1R (all), TAD level:not found; TUBB3 (all), TAD level:not found</t>
+  </si>
+  <si>
+    <t>ALS2 (hacat_unstim_2, hacat_unstim only), TAD level:1; NOP58 (hacat_unstim_2, hacat_unstim only), TAD level:not found; CASP8 (all), TAD level:not found; STRADB (hacat_unstim_2, hacat_unstim only), TAD level:2; TRAK2 (hacat_unstim_2 only), TAD level:2; TMEM237 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>MTAP (all), TAD level:2; CDKN2A (hacat_unstim_2, hacat_unstim only), TAD level:3; KLHL9 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>APOLD1 (myla_1, myla only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>DUSP22 (myla_1, myla only), TAD level:1; EXOC2 (myla_1, myla only), TAD level:1</t>
+  </si>
+  <si>
+    <t>SEC62 (myla_1, myla only), TAD level:1; MYNN (all), TAD level:not found; SKIL (all), TAD level:1; PRKCI (myla only), TAD level:1; RPL22L1 (all), TAD level:not found; PHC3 (myla_2, myla only), TAD level:1; GPR160 (myla_1 only), TAD level:1; ACTRT3 (all), TAD level:not found</t>
+  </si>
+  <si>
+    <t>CBY1 (myla_1, myla only), TAD level:2; TOMM22 (myla only), TAD level:2; JOSD1 (myla_1, myla only), TAD level:2; PLA2G6 (all), TAD level:2; FAM227A (myla_1, myla only), TAD level:2; CSNK1E (myla only), TAD level:2</t>
   </si>
   <si>
     <t>TARS (all), TAD level:not found</t>
   </si>
   <si>
-    <t>PARP1 (all), TAD level:1; ACBD3 (myla_1,myla only), TAD level:1</t>
-  </si>
-  <si>
-    <t>CLPTM1L (all), TAD level:1; LPCAT1 (myla_1,myla only), TAD level:2</t>
+    <t>PARP1 (all), TAD level:1; ACBD3 (myla_1, myla only), TAD level:1</t>
+  </si>
+  <si>
+    <t>CLPTM1L (all), TAD level:1; LPCAT1 (myla_1, myla only), TAD level:2</t>
   </si>
   <si>
     <t>MX2 (all), TAD level:3</t>
@@ -530,46 +530,46 @@
     <t>GDI2 (all), TAD level:1; NET1 (myla only), TAD level:not found</t>
   </si>
   <si>
-    <t>TP53INP2 (all), TAD level:2; EDEM2 (myla only), TAD level:2; TRPC4AP (myla_2,myla only), TAD level:2; AHCY (myla_2,myla only), TAD level:1; PIGU (all), TAD level:2; CEP250 (myla only), TAD level:2; MMP24OS (all), TAD level:1; EIF6 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>PRPF3 (myla only), TAD level:3; APH1A (all), TAD level:1; TARS2 (all), TAD level:3; SETDB1 (myla_1,myla only), TAD level:4; MCL1 (all), TAD level:3; ANP32E (all), TAD level:1; CERS2 (all), TAD level:4; ENSA (all), TAD level:4; ARNT (myla only), TAD level:4; GOLPH3L (all), TAD level:4; RPRD2 (all), TAD level:3; MRPS21 (myla_1,myla only), TAD level:3</t>
-  </si>
-  <si>
-    <t>ACAT1 (myla only), TAD level:3; ZC3H12C (myla only), TAD level:2; NPAT (myla_1,myla only), TAD level:3; ATM (myla_1,myla only), TAD level:3; DDX10 (myla_1,myla only), TAD level:2</t>
+    <t>TP53INP2 (all), TAD level:2; EDEM2 (myla only), TAD level:2; TRPC4AP (myla_2, myla only), TAD level:2; AHCY (myla_2, myla only), TAD level:1; PIGU (all), TAD level:2; CEP250 (myla only), TAD level:2; MMP24OS (all), TAD level:1; EIF6 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>PRPF3 (myla only), TAD level:3; APH1A (all), TAD level:1; TARS2 (all), TAD level:3; SETDB1 (myla_1, myla only), TAD level:4; MCL1 (all), TAD level:3; ANP32E (all), TAD level:1; CERS2 (all), TAD level:4; ENSA (all), TAD level:4; ARNT (myla only), TAD level:4; GOLPH3L (all), TAD level:4; RPRD2 (all), TAD level:3; MRPS21 (myla_1, myla only), TAD level:3</t>
+  </si>
+  <si>
+    <t>ACAT1 (myla only), TAD level:3; ZC3H12C (myla only), TAD level:2; NPAT (myla_1, myla only), TAD level:3; ATM (myla_1, myla only), TAD level:3; DDX10 (myla_1, myla only), TAD level:2</t>
   </si>
   <si>
     <t>TMTC3 (myla only), TAD level:1; CEP290 (myla only), TAD level:not found</t>
   </si>
   <si>
-    <t>TCF25 (myla_1,myla only), TAD level:not found; ZNF778 (myla_2,myla only), TAD level:not found; CPNE7 (all), TAD level:not found</t>
-  </si>
-  <si>
-    <t>ALS2 (all), TAD level:1; NOP58 (myla_2,myla only), TAD level:not found; CASP8 (all), TAD level:not found; TMEM237 (all), TAD level:2</t>
+    <t>TCF25 (myla_1, myla only), TAD level:not found; ZNF778 (myla_2, myla only), TAD level:not found; CPNE7 (all), TAD level:not found</t>
+  </si>
+  <si>
+    <t>ALS2 (all), TAD level:1; NOP58 (myla_2, myla only), TAD level:not found; CASP8 (all), TAD level:not found; TMEM237 (all), TAD level:2</t>
   </si>
   <si>
     <t>MTAP (myla only), TAD level:not found; KLHL9 (myla only), TAD level:1</t>
   </si>
   <si>
-    <t>SEC62 (all); MYNN (all); SKIL (all); TNIK (all); PRKCI (all); EIF5A2 (all); RPL22L1 (all); LRRC34 (naive_T_2,naive_T only); PHC3 (all); GPR160 (all)</t>
-  </si>
-  <si>
-    <t>JOSD1 (naive_T_1,naive_T only); PLA2G6 (all); MAFF (all)</t>
-  </si>
-  <si>
-    <t>SYNE2 (naive_T_1,naive_T only)</t>
+    <t>SEC62 (all); MYNN (all); SKIL (all); TNIK (all); PRKCI (all); EIF5A2 (all); RPL22L1 (all); LRRC34 (naive_T_2, naive_T only); PHC3 (all); GPR160 (all)</t>
+  </si>
+  <si>
+    <t>JOSD1 (naive_T_1, naive_T only); PLA2G6 (all); MAFF (all)</t>
+  </si>
+  <si>
+    <t>SYNE2 (naive_T_1, naive_T only)</t>
   </si>
   <si>
     <t>PARP1 (all)</t>
   </si>
   <si>
-    <t>CLPTM1L (all); SLC12A7 (naive_T_2,naive_T only)</t>
-  </si>
-  <si>
-    <t>MX1 (naive_T_1,naive_T only); MX2 (all)</t>
-  </si>
-  <si>
-    <t>GDI2 (all); FAM208B (all); NET1 (naive_T_2,naive_T only); ASB13 (naive_T only)</t>
+    <t>CLPTM1L (all); SLC12A7 (naive_T_2, naive_T only)</t>
+  </si>
+  <si>
+    <t>MX1 (naive_T_1, naive_T only); MX2 (all)</t>
+  </si>
+  <si>
+    <t>GDI2 (all); FAM208B (all); NET1 (naive_T_2, naive_T only); ASB13 (naive_T only)</t>
   </si>
   <si>
     <t>TPCN2 (naive_T_1 only)</t>
@@ -578,22 +578,22 @@
     <t>HDAC4 (all)</t>
   </si>
   <si>
-    <t>PHF20 (naive_T_1,naive_T only); EDEM2 (naive_T only); GSS (all); TRPC4AP (all); AHCY (naive_T only); DYNLRB1 (naive_T only); MMP24OS (all); CNBD2 (naive_T only); SCAND1 (naive_T only); EIF6 (all)</t>
-  </si>
-  <si>
-    <t>DOCK8 (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>PRPF3 (naive_T_2,naive_T only); APH1A (naive_T only); C1orf54 (naive_T only); CA14 (naive_T only); PRUNE1 (all); SF3B4 (naive_T only); ANP32E (naive_T_1 only); MINDY1 (all); CERS2 (all); ENSA (naive_T_1,naive_T only); ARNT (naive_T only); GOLPH3L (all); RPRD2 (all); CTSS (all); TNFAIP8L2 (naive_T_2 only); SCNM1 (naive_T_2 only)</t>
-  </si>
-  <si>
-    <t>ACAT1 (all); EXPH5 (all); ALKBH8 (naive_T_2,naive_T only); NPAT (all); ATM (all); CWF19L2 (naive_T_2,naive_T only); CUL5 (naive_T_1,naive_T only); C11orf65 (all); DDX10 (all); KDELC2 (all)</t>
-  </si>
-  <si>
-    <t>VPS9D1 (naive_T_2 only); TCF25 (all); RNF166 (naive_T only); SPATA2L (all); ZNF276 (naive_T_2 only); ANKRD11 (naive_T_2,naive_T only); ZNF778 (all); CTU2 (naive_T only); CDK10 (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>ALS2 (all); CLK1 (all); NOP58 (all); CASP8 (all); STRADB (all); BZW1 (naive_T_1,naive_T only); TRAK2 (all); SUMO1 (naive_T_2,naive_T only); CYP20A1 (naive_T_2,naive_T only); FAM117B (naive_T_2,naive_T only); TMEM237 (all); NIF3L1 (all); BMPR2 (naive_T_2,naive_T only); PPIL3 (all)</t>
+    <t>PHF20 (naive_T_1, naive_T only); EDEM2 (naive_T only); GSS (all); TRPC4AP (all); AHCY (naive_T only); DYNLRB1 (naive_T only); MMP24OS (all); CNBD2 (naive_T only); SCAND1 (naive_T only); EIF6 (all)</t>
+  </si>
+  <si>
+    <t>DOCK8 (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>PRPF3 (naive_T_2, naive_T only); APH1A (naive_T only); C1orf54 (naive_T only); CA14 (naive_T only); PRUNE1 (all); SF3B4 (naive_T only); ANP32E (naive_T_1 only); MINDY1 (all); CERS2 (all); ENSA (naive_T_1, naive_T only); ARNT (naive_T only); GOLPH3L (all); RPRD2 (all); CTSS (all); TNFAIP8L2 (naive_T_2 only); SCNM1 (naive_T_2 only)</t>
+  </si>
+  <si>
+    <t>ACAT1 (all); EXPH5 (all); ALKBH8 (naive_T_2, naive_T only); NPAT (all); ATM (all); CWF19L2 (naive_T_2, naive_T only); CUL5 (naive_T_1, naive_T only); C11orf65 (all); DDX10 (all); KDELC2 (all)</t>
+  </si>
+  <si>
+    <t>VPS9D1 (naive_T_2 only); TCF25 (all); RNF166 (naive_T only); SPATA2L (all); ZNF276 (naive_T_2 only); ANKRD11 (naive_T_2, naive_T only); ZNF778 (all); CTU2 (naive_T only); CDK10 (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>ALS2 (all); CLK1 (all); NOP58 (all); CASP8 (all); STRADB (all); BZW1 (naive_T_1, naive_T only); TRAK2 (all); SUMO1 (naive_T_2, naive_T only); CYP20A1 (naive_T_2, naive_T only); FAM117B (naive_T_2, naive_T only); TMEM237 (all); NIF3L1 (all); BMPR2 (naive_T_2, naive_T only); PPIL3 (all)</t>
   </si>
   <si>
     <t>MTAP (all); KLHL9 (naive_T only)</t>
@@ -770,7 +770,7 @@
     <t>ID2 (hacat_stim only), TAD level:2</t>
   </si>
   <si>
-    <t>RAD1 (hacat_stim_2,hacat_stim only), TAD level:outside tad; BRIX1 (hacat_stim_2,hacat_stim only), TAD level:outside tad; IL7R (all), TAD level:1; DNAJC21 (all), TAD level:outside tad</t>
+    <t>RAD1 (hacat_stim_2, hacat_stim only), TAD level:outside tad; BRIX1 (hacat_stim_2, hacat_stim only), TAD level:outside tad; IL7R (all), TAD level:1; DNAJC21 (all), TAD level:outside tad</t>
   </si>
   <si>
     <t>SSH3 (hacat_stim only), TAD level:outside tad; RNASEH2C (hacat_stim_1 only), TAD level:2; KAT5 (all), TAD level:2</t>
@@ -779,49 +779,49 @@
     <t>ATP6V1B1 (hacat_stim only), TAD level:not found</t>
   </si>
   <si>
-    <t>SEPT8 (hacat_stim_2,hacat_stim only), TAD level:2; UQCRQ (hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>EFNA3 (hacat_stim only), TAD level:outside tad; ZBTB7B (hacat_stim only), TAD level:outside tad; SHC1 (hacat_stim_2,hacat_stim only), TAD level:not found; IL6R (hacat_stim_2,hacat_stim only), TAD level:2; CKS1B (hacat_stim_2,hacat_stim only), TAD level:not found; S100A16 (hacat_stim_2 only), TAD level:outside tad; S100A14 (hacat_stim_2 only), TAD level:outside tad; S100A2 (hacat_stim_2,hacat_stim only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>ATP6V0A1 (hacat_stim_2,hacat_stim only), TAD level:2; STAT3 (hacat_stim_2,hacat_stim only), TAD level:3; CAVIN1 (all), TAD level:4</t>
-  </si>
-  <si>
-    <t>PPP2R3C (all), TAD level:2; SRP54 (hacat_stim_2,hacat_stim only), TAD level:2; KIAA0391 (all), TAD level:2; PSMA6 (all), TAD level:3; NFKBIA (all), TAD level:1; SNX6 (hacat_stim only), TAD level:not found; FAM177A1 (all), TAD level:2; CFL2 (hacat_stim_2,hacat_stim only), TAD level:2; RALGAPA1 (hacat_stim only), TAD level:not found; BAZ1A (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>EMSY (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>EGR2 (hacat_stim_2,hacat_stim only), TAD level:1; ADO (hacat_stim_2,hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>REL (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>PTK6 (all), TAD level:3; GMEB2 (hacat_stim_2,hacat_stim only), TAD level:3; SLC2A4RG (hacat_stim only), TAD level:3; TCEA2 (hacat_stim only), TAD level:3; STMN3 (all), TAD level:3; UCKL1 (hacat_stim only), TAD level:3</t>
+    <t>SEPT8 (hacat_stim_2, hacat_stim only), TAD level:2; UQCRQ (hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>EFNA3 (hacat_stim only), TAD level:outside tad; ZBTB7B (hacat_stim only), TAD level:outside tad; SHC1 (hacat_stim_2, hacat_stim only), TAD level:not found; IL6R (hacat_stim_2, hacat_stim only), TAD level:2; CKS1B (hacat_stim_2, hacat_stim only), TAD level:not found; S100A16 (hacat_stim_2 only), TAD level:outside tad; S100A14 (hacat_stim_2 only), TAD level:outside tad; S100A2 (hacat_stim_2, hacat_stim only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>ATP6V0A1 (hacat_stim_2, hacat_stim only), TAD level:2; STAT3 (hacat_stim_2, hacat_stim only), TAD level:3; CAVIN1 (all), TAD level:4</t>
+  </si>
+  <si>
+    <t>PPP2R3C (all), TAD level:2; SRP54 (hacat_stim_2, hacat_stim only), TAD level:2; KIAA0391 (all), TAD level:2; PSMA6 (all), TAD level:3; NFKBIA (all), TAD level:1; SNX6 (hacat_stim only), TAD level:not found; FAM177A1 (all), TAD level:2; CFL2 (hacat_stim_2, hacat_stim only), TAD level:2; RALGAPA1 (hacat_stim only), TAD level:not found; BAZ1A (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>EMSY (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>EGR2 (hacat_stim_2, hacat_stim only), TAD level:1; ADO (hacat_stim_2, hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>REL (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>PTK6 (all), TAD level:3; GMEB2 (hacat_stim_2, hacat_stim only), TAD level:3; SLC2A4RG (hacat_stim only), TAD level:3; TCEA2 (hacat_stim only), TAD level:3; STMN3 (all), TAD level:3; UCKL1 (hacat_stim only), TAD level:3</t>
   </si>
   <si>
     <t>IL18R1 (all), TAD level:3</t>
   </si>
   <si>
-    <t>APH1A (hacat_stim_2,hacat_stim only), TAD level:not found; C1orf54 (hacat_stim_2,hacat_stim only), TAD level:not found; PRUNE1 (all), TAD level:not found; TARS2 (all), TAD level:2; SETDB1 (hacat_stim only), TAD level:2; PIP5K1A (hacat_stim_2,hacat_stim only), TAD level:outside tad; MINDY1 (all), TAD level:not found; ANXA9 (all), TAD level:2; CERS2 (all), TAD level:2; ARNT (all), TAD level:2; GABPB2 (all), TAD level:not found; CIART (hacat_stim_2,hacat_stim only), TAD level:2; VPS72 (hacat_stim_2,hacat_stim only), TAD level:outside tad; CDC42SE1 (all), TAD level:not found; MRPS21 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>NEK4 (hacat_stim_2,hacat_stim only), TAD level:not found; PRKCD (hacat_stim only), TAD level:1; SFMBT1 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>ID2 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>RAD1 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; BRIX1 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; IL7R (all), TAD level:1; DNAJC21 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>RNASEH2C (hacat_unstim_2 only), TAD level:3; KAT5 (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>TEX261 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
+    <t>APH1A (hacat_stim_2, hacat_stim only), TAD level:not found; C1orf54 (hacat_stim_2, hacat_stim only), TAD level:not found; PRUNE1 (all), TAD level:not found; TARS2 (all), TAD level:2; SETDB1 (hacat_stim only), TAD level:2; PIP5K1A (hacat_stim_2, hacat_stim only), TAD level:outside tad; MINDY1 (all), TAD level:not found; ANXA9 (all), TAD level:2; CERS2 (all), TAD level:2; ARNT (all), TAD level:2; GABPB2 (all), TAD level:not found; CIART (hacat_stim_2, hacat_stim only), TAD level:2; VPS72 (hacat_stim_2, hacat_stim only), TAD level:outside tad; CDC42SE1 (all), TAD level:not found; MRPS21 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>NEK4 (hacat_stim_2, hacat_stim only), TAD level:not found; PRKCD (hacat_stim only), TAD level:1; SFMBT1 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>ID2 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>RAD1 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; BRIX1 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; IL7R (all), TAD level:1; DNAJC21 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>RNASEH2C (hacat_unstim_2 only), TAD level:3; KAT5 (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>TEX261 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
   </si>
   <si>
     <t>P4HA2 (hacat_unstim_2 only), TAD level:1; UQCRQ (hacat_unstim_2 only), TAD level:2; LEAP2 (hacat_unstim_2 only), TAD level:2; SLC22A4 (hacat_unstim_2 only), TAD level:1</t>
@@ -830,91 +830,91 @@
     <t>GTPBP8 (hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
-    <t>SHC1 (all), TAD level:not found; IL6R (all), TAD level:1; EFNA1 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; CKS1B (all), TAD level:not found; S100A16 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; S100A14 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>ATP6V0A1 (all), TAD level:1; COASY (all), TAD level:1; HSD17B1 (hacat_unstim only), TAD level:1; MLX (all), TAD level:1; PSMC3IP (hacat_unstim_2,hacat_unstim only), TAD level:1; STAT3 (hacat_unstim_2,hacat_unstim only), TAD level:1; CAVIN1 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>PPP2R3C (all), TAD level:2; SRP54 (hacat_unstim_2,hacat_unstim only), TAD level:3; KIAA0391 (all), TAD level:2; PSMA6 (all), TAD level:3; NFKBIA (all), TAD level:1; SNX6 (hacat_unstim only), TAD level:not found; FAM177A1 (all), TAD level:2; CFL2 (hacat_unstim only), TAD level:3; BAZ1A (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>ADO (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>PRPF6 (hacat_unstim only), TAD level:3; PTK6 (all), TAD level:3; GMEB2 (hacat_unstim_2,hacat_unstim only), TAD level:3; ARFRP1 (hacat_unstim_2,hacat_unstim only), TAD level:3; PPDPF (hacat_unstim only), TAD level:3; SAMD10 (hacat_unstim only), TAD level:3; TCEA2 (hacat_unstim only), TAD level:3; STMN3 (all), TAD level:3</t>
-  </si>
-  <si>
-    <t>IL18R1 (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>PRUNE1 (all), TAD level:2; ECM1 (hacat_unstim only), TAD level:4; TARS2 (all), TAD level:4; SETDB1 (hacat_unstim_2,hacat_unstim only), TAD level:4; PIP5K1A (hacat_unstim_2,hacat_unstim only), TAD level:not found; ANP32E (hacat_unstim_2,hacat_unstim only), TAD level:2; MINDY1 (all), TAD level:2; ANXA9 (all), TAD level:4; CERS2 (all), TAD level:4; ARNT (hacat_unstim_2,hacat_unstim only), TAD level:4; C1orf56 (hacat_unstim_2,hacat_unstim only), TAD level:2; GABPB2 (hacat_unstim only), TAD level:2; CIART (hacat_unstim_2,hacat_unstim only), TAD level:1; VPS72 (hacat_unstim_2,hacat_unstim only), TAD level:2; CDC42SE1 (hacat_unstim only), TAD level:2; MRPS21 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>PRKCD (all), TAD level:1; SFMBT1 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>RAD1 (myla_1,myla only), TAD level:outside tad; BRIX1 (myla_1,myla only), TAD level:outside tad; PRLR (myla_1,myla only), TAD level:not found; SPEF2 (all), TAD level:1; IL7R (all), TAD level:2; DNAJC21 (myla_1,myla only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>RNASEH2C (myla only), TAD level:2; KAT5 (myla_1,myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>FAM136A (myla_1,myla only), TAD level:2; SNRPG (myla only), TAD level:2</t>
+    <t>SHC1 (all), TAD level:not found; IL6R (all), TAD level:1; EFNA1 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; CKS1B (all), TAD level:not found; S100A16 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; S100A14 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>ATP6V0A1 (all), TAD level:1; COASY (all), TAD level:1; HSD17B1 (hacat_unstim only), TAD level:1; MLX (all), TAD level:1; PSMC3IP (hacat_unstim_2, hacat_unstim only), TAD level:1; STAT3 (hacat_unstim_2, hacat_unstim only), TAD level:1; CAVIN1 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>PPP2R3C (all), TAD level:2; SRP54 (hacat_unstim_2, hacat_unstim only), TAD level:3; KIAA0391 (all), TAD level:2; PSMA6 (all), TAD level:3; NFKBIA (all), TAD level:1; SNX6 (hacat_unstim only), TAD level:not found; FAM177A1 (all), TAD level:2; CFL2 (hacat_unstim only), TAD level:3; BAZ1A (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>ADO (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>PRPF6 (hacat_unstim only), TAD level:3; PTK6 (all), TAD level:3; GMEB2 (hacat_unstim_2, hacat_unstim only), TAD level:3; ARFRP1 (hacat_unstim_2, hacat_unstim only), TAD level:3; PPDPF (hacat_unstim only), TAD level:3; SAMD10 (hacat_unstim only), TAD level:3; TCEA2 (hacat_unstim only), TAD level:3; STMN3 (all), TAD level:3</t>
+  </si>
+  <si>
+    <t>IL18R1 (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>PRUNE1 (all), TAD level:2; ECM1 (hacat_unstim only), TAD level:4; TARS2 (all), TAD level:4; SETDB1 (hacat_unstim_2, hacat_unstim only), TAD level:4; PIP5K1A (hacat_unstim_2, hacat_unstim only), TAD level:not found; ANP32E (hacat_unstim_2, hacat_unstim only), TAD level:2; MINDY1 (all), TAD level:2; ANXA9 (all), TAD level:4; CERS2 (all), TAD level:4; ARNT (hacat_unstim_2, hacat_unstim only), TAD level:4; C1orf56 (hacat_unstim_2, hacat_unstim only), TAD level:2; GABPB2 (hacat_unstim only), TAD level:2; CIART (hacat_unstim_2, hacat_unstim only), TAD level:1; VPS72 (hacat_unstim_2, hacat_unstim only), TAD level:2; CDC42SE1 (hacat_unstim only), TAD level:2; MRPS21 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>PRKCD (all), TAD level:1; SFMBT1 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>RAD1 (myla_1, myla only), TAD level:outside tad; BRIX1 (myla_1, myla only), TAD level:outside tad; PRLR (myla_1, myla only), TAD level:not found; SPEF2 (all), TAD level:1; IL7R (all), TAD level:2; DNAJC21 (myla_1, myla only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>RNASEH2C (myla only), TAD level:2; KAT5 (myla_1, myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>FAM136A (myla_1, myla only), TAD level:2; SNRPG (myla only), TAD level:2</t>
   </si>
   <si>
     <t>RAD50 (all), TAD level:1; IL5 (all), TAD level:1; KIF3A (all), TAD level:2; SEPT8 (all), TAD level:2; SHROOM1 (all), TAD level:2; IL13 (all), TAD level:2</t>
   </si>
   <si>
-    <t>ATP8B2 (myla_1,myla only), TAD level:4; SHC1 (myla_2,myla only), TAD level:2; CKS1B (myla_2,myla only), TAD level:2</t>
+    <t>ATP8B2 (myla_1, myla only), TAD level:4; SHC1 (myla_2, myla only), TAD level:2; CKS1B (myla_2, myla only), TAD level:2</t>
   </si>
   <si>
     <t>STAT3 (myla_2 only), TAD level:3</t>
   </si>
   <si>
-    <t>PPP2R3C (all), TAD level:2; KIAA0391 (all), TAD level:2; PSMA6 (all), TAD level:3; NFKBIA (all), TAD level:1; SNX6 (myla_1,myla only), TAD level:not found; FAM177A1 (all), TAD level:2; CFL2 (myla_1,myla only), TAD level:2; RALGAPA1 (myla only), TAD level:1; BAZ1A (myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>PRR5L (myla_1,myla only), TAD level:not found; TRAF6 (myla only), TAD level:1</t>
-  </si>
-  <si>
-    <t>ZNF846 (myla_1,myla only), TAD level:1</t>
-  </si>
-  <si>
-    <t>NRBF2 (myla_1,myla only), TAD level:not found; ADO (myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>TPD52L2 (myla only), TAD level:3; PTK6 (myla only), TAD level:3; C20orf204 (myla_1,myla only), TAD level:3; STMN3 (all), TAD level:3</t>
+    <t>PPP2R3C (all), TAD level:2; KIAA0391 (all), TAD level:2; PSMA6 (all), TAD level:3; NFKBIA (all), TAD level:1; SNX6 (myla_1, myla only), TAD level:not found; FAM177A1 (all), TAD level:2; CFL2 (myla_1, myla only), TAD level:2; RALGAPA1 (myla only), TAD level:1; BAZ1A (myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>PRR5L (myla_1, myla only), TAD level:not found; TRAF6 (myla only), TAD level:1</t>
+  </si>
+  <si>
+    <t>ZNF846 (myla_1, myla only), TAD level:1</t>
+  </si>
+  <si>
+    <t>NRBF2 (myla_1, myla only), TAD level:not found; ADO (myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>TPD52L2 (myla only), TAD level:3; PTK6 (myla only), TAD level:3; C20orf204 (myla_1, myla only), TAD level:3; STMN3 (all), TAD level:3</t>
   </si>
   <si>
     <t>IL18R1 (all), TAD level:2</t>
   </si>
   <si>
-    <t>IL15RA (myla_1,myla only), TAD level:2</t>
+    <t>IL15RA (myla_1, myla only), TAD level:2</t>
   </si>
   <si>
     <t>ETS1 (all), TAD level:2</t>
   </si>
   <si>
-    <t>PRPF3 (myla only), TAD level:4; APH1A (myla_1,myla only), TAD level:1; PRUNE1 (myla_1,myla only), TAD level:2; TARS2 (all), TAD level:4; CERS2 (all), TAD level:4; GABPB2 (myla only), TAD level:2; CDC42SE1 (myla only), TAD level:2; MRPS21 (all), TAD level:4</t>
-  </si>
-  <si>
-    <t>NEK4 (myla_1,myla only), TAD level:not found; PRKCD (myla_1,myla only), TAD level:2; TMEM110-MUSTN1 (myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>WDR70 (naive_T_2,naive_T only); RAD1 (all); BRIX1 (all); NUP155 (naive_T_2,naive_T only); SPEF2 (all); NADK2 (naive_T_1,naive_T only); NIPBL (all); IL7R (all); DNAJC21 (all)</t>
+    <t>PRPF3 (myla only), TAD level:4; APH1A (myla_1, myla only), TAD level:1; PRUNE1 (myla_1, myla only), TAD level:2; TARS2 (all), TAD level:4; CERS2 (all), TAD level:4; GABPB2 (myla only), TAD level:2; CDC42SE1 (myla only), TAD level:2; MRPS21 (all), TAD level:4</t>
+  </si>
+  <si>
+    <t>NEK4 (myla_1, myla only), TAD level:not found; PRKCD (myla_1, myla only), TAD level:2; TMEM110-MUSTN1 (myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>WDR70 (naive_T_2, naive_T only); RAD1 (all); BRIX1 (all); NUP155 (naive_T_2, naive_T only); SPEF2 (all); NADK2 (naive_T_1, naive_T only); NIPBL (all); IL7R (all); DNAJC21 (all)</t>
   </si>
   <si>
     <t>KAT5 (naive_T only); SART1 (naive_T_1 only)</t>
   </si>
   <si>
-    <t>AFF4 (naive_T_1,naive_T only); PPP2CA (naive_T only); C5orf15 (naive_T_1 only); RAPGEF6 (naive_T only); UQCRQ (all); LEAP2 (all); HSPA4 (all); SLC22A5 (naive_T_2,naive_T only); AC104109.3 (naive_T only)</t>
+    <t>AFF4 (naive_T_1, naive_T only); PPP2CA (naive_T only); C5orf15 (naive_T_1 only); RAPGEF6 (naive_T only); UQCRQ (all); LEAP2 (all); HSPA4 (all); SLC22A5 (naive_T_2, naive_T only); AC104109.3 (naive_T only)</t>
   </si>
   <si>
     <t>ADAM15 (naive_T only); IL6R (all); PMVK (naive_T only); PBXIP1 (all); PYGO2 (all)</t>
   </si>
   <si>
-    <t>NAGLU (naive_T_2 only); HSD17B1 (naive_T_2 only); GHDC (naive_T_1,naive_T only); STAT3 (all)</t>
+    <t>NAGLU (naive_T_2 only); HSD17B1 (naive_T_2 only); GHDC (naive_T_1, naive_T only); STAT3 (all)</t>
   </si>
   <si>
     <t>PPP2R3C (all); SRP54 (all); KIAA0391 (all); PSMA6 (all); NFKBIA (all); BRMS1L (all); SNX6 (all); EAPP (all); FAM177A1 (all); MBIP (naive_T only); CFL2 (all); RALGAPA1 (all); BAZ1A (all)</t>
@@ -935,13 +935,13 @@
     <t>EXOSC9 (all); BBS7 (all); KIAA1109 (naive_T only)</t>
   </si>
   <si>
-    <t>ETS1 (all); FLI1 (naive_T_1,naive_T only); TMEM45B (naive_T_1 only)</t>
-  </si>
-  <si>
-    <t>APH1A (naive_T_1,naive_T only); C1orf54 (naive_T_1,naive_T only); CA14 (naive_T_1,naive_T only); PRUNE1 (all); SF3B4 (naive_T_2,naive_T only); PIP5K1A (naive_T_1,naive_T only); MINDY1 (all); ANXA9 (all); CERS2 (all); ENSA (naive_T only); ARNT (naive_T only); GOLPH3L (naive_T_1,naive_T only); GABPB2 (all); CIART (all); TNFAIP8L2 (naive_T_2 only); LYSMD1 (naive_T only); SCNM1 (naive_T_2,naive_T only); TMOD4 (naive_T only); VPS72 (naive_T_1,naive_T only); BOLA1 (naive_T only); HIST2H2AC (naive_T only); HIST2H2BE (naive_T only); CDC42SE1 (all); MLLT11 (naive_T only); MRPS21 (all)</t>
-  </si>
-  <si>
-    <t>SELENOK (all); ACTR8 (all); NEK4 (naive_T_1 only); TKT (naive_T_1,naive_T only); PRKCD (all); SFMBT1 (all); GNL3 (all); PBRM1 (all); STIMATE (all); TMEM110-MUSTN1 (all)</t>
+    <t>ETS1 (all); FLI1 (naive_T_1, naive_T only); TMEM45B (naive_T_1 only)</t>
+  </si>
+  <si>
+    <t>APH1A (naive_T_1, naive_T only); C1orf54 (naive_T_1, naive_T only); CA14 (naive_T_1, naive_T only); PRUNE1 (all); SF3B4 (naive_T_2, naive_T only); PIP5K1A (naive_T_1, naive_T only); MINDY1 (all); ANXA9 (all); CERS2 (all); ENSA (naive_T only); ARNT (naive_T only); GOLPH3L (naive_T_1, naive_T only); GABPB2 (all); CIART (all); TNFAIP8L2 (naive_T_2 only); LYSMD1 (naive_T only); SCNM1 (naive_T_2, naive_T only); TMOD4 (naive_T only); VPS72 (naive_T_1, naive_T only); BOLA1 (naive_T only); HIST2H2AC (naive_T only); HIST2H2BE (naive_T only); CDC42SE1 (all); MLLT11 (naive_T only); MRPS21 (all)</t>
+  </si>
+  <si>
+    <t>SELENOK (all); ACTR8 (all); NEK4 (naive_T_1 only); TKT (naive_T_1, naive_T only); PRKCD (all); SFMBT1 (all); GNL3 (all); PBRM1 (all); STIMATE (all); TMEM110-MUSTN1 (all)</t>
   </si>
   <si>
     <t>rs1005714</t>
@@ -1148,109 +1148,109 @@
     <t>ARHGAP31; COX17; POGLUT1; TMEM39A</t>
   </si>
   <si>
-    <t>LLGL2 (hacat_stim_2,hacat_stim only), TAD level:3; CDR2L (all), TAD level:not found; MRPS7 (all), TAD level:not found; GGA3 (all), TAD level:not found; ARMC7 (all), TAD level:1; NUP85 (all), TAD level:1; SLC25A19 (hacat_stim_2 only), TAD level:not found; MIF4GD (all), TAD level:not found; NT5C (hacat_stim only), TAD level:1; ATP5PD (all), TAD level:1; CASKIN2 (hacat_stim_2,hacat_stim only), TAD level:3; GRB2 (all), TAD level:not found; KCTD2 (all), TAD level:1; TSEN54 (hacat_stim_2,hacat_stim only), TAD level:3</t>
+    <t>LLGL2 (hacat_stim_2, hacat_stim only), TAD level:3; CDR2L (all), TAD level:not found; MRPS7 (all), TAD level:not found; GGA3 (all), TAD level:not found; ARMC7 (all), TAD level:1; NUP85 (all), TAD level:1; SLC25A19 (hacat_stim_2 only), TAD level:not found; MIF4GD (all), TAD level:not found; NT5C (hacat_stim only), TAD level:1; ATP5PD (all), TAD level:1; CASKIN2 (hacat_stim_2, hacat_stim only), TAD level:3; GRB2 (all), TAD level:not found; KCTD2 (all), TAD level:1; TSEN54 (hacat_stim_2, hacat_stim only), TAD level:3</t>
   </si>
   <si>
     <t>DDX6 (all), TAD level:2; UPK2 (hacat_stim only), TAD level:2; CCDC84 (hacat_stim only), TAD level:2; BCL9L (all), TAD level:2</t>
   </si>
   <si>
-    <t>DGKQ (all), TAD level:not found; ATP5ME (hacat_stim_2,hacat_stim only), TAD level:not found; GAK (hacat_stim_2,hacat_stim only), TAD level:1; MYL5 (hacat_stim_2,hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>IRF5 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>CSK (all), TAD level:4; ULK3 (hacat_stim_2 only), TAD level:4; C15orf39 (hacat_stim_2,hacat_stim only), TAD level:2; RPP25 (hacat_stim_2,hacat_stim only), TAD level:4; COX5A (hacat_stim_2,hacat_stim only), TAD level:4; FAM219B (all), TAD level:4</t>
-  </si>
-  <si>
-    <t>NAB1 (all), TAD level:1; INPP1 (all), TAD level:not found; MFSD6 (hacat_stim_2,hacat_stim only), TAD level:1; NEMP2 (all), TAD level:1; HIBCH (all), TAD level:not found</t>
-  </si>
-  <si>
-    <t>DARS2 (hacat_stim_2,hacat_stim only), TAD level:not found; CENPL (hacat_stim_2,hacat_stim only), TAD level:not found</t>
+    <t>DGKQ (all), TAD level:not found; ATP5ME (hacat_stim_2, hacat_stim only), TAD level:not found; GAK (hacat_stim_2, hacat_stim only), TAD level:1; MYL5 (hacat_stim_2, hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>IRF5 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>CSK (all), TAD level:4; ULK3 (hacat_stim_2 only), TAD level:4; C15orf39 (hacat_stim_2, hacat_stim only), TAD level:2; RPP25 (hacat_stim_2, hacat_stim only), TAD level:4; COX5A (hacat_stim_2, hacat_stim only), TAD level:4; FAM219B (all), TAD level:4</t>
+  </si>
+  <si>
+    <t>NAB1 (all), TAD level:1; INPP1 (all), TAD level:not found; MFSD6 (hacat_stim_2, hacat_stim only), TAD level:1; NEMP2 (all), TAD level:1; HIBCH (all), TAD level:not found</t>
+  </si>
+  <si>
+    <t>DARS2 (hacat_stim_2, hacat_stim only), TAD level:not found; CENPL (hacat_stim_2, hacat_stim only), TAD level:not found</t>
   </si>
   <si>
     <t>PRDX6 (hacat_stim only), TAD level:5</t>
   </si>
   <si>
-    <t>POU2F1 (hacat_stim_2,hacat_stim only), TAD level:2; TADA1 (hacat_stim only), TAD level:not found</t>
+    <t>POU2F1 (hacat_stim_2, hacat_stim only), TAD level:2; TADA1 (hacat_stim only), TAD level:not found</t>
   </si>
   <si>
     <t>NFKB1 (all), TAD level:1; UBE2D3 (all), TAD level:1; CISD2 (hacat_stim only), TAD level:1</t>
   </si>
   <si>
-    <t>CD81 (hacat_stim only), TAD level:4; TSSC4 (hacat_stim_2,hacat_stim only), TAD level:4</t>
-  </si>
-  <si>
-    <t>TNPO3 (hacat_stim_2,hacat_stim only), TAD level:2; IRF5 (hacat_stim_2,hacat_stim only), TAD level:2; KCP (hacat_stim_2,hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>GADD45A (hacat_stim_2 only), TAD level:outside tad; SERBP1 (hacat_stim_2,hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>NDST1 (hacat_stim only), TAD level:1; TNIP1 (hacat_stim only), TAD level:2; SYNPO (hacat_stim_2,hacat_stim only), TAD level:1; ATOX1 (hacat_stim_2 only), TAD level:not found; GM2A (hacat_stim_2 only), TAD level:2</t>
-  </si>
-  <si>
-    <t>STAT1 (hacat_stim_2,hacat_stim only), TAD level:not found; MFSD6 (hacat_stim_2,hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>IFT80 (hacat_stim_2,hacat_stim only), TAD level:2; SMC4 (hacat_stim_2,hacat_stim only), TAD level:not found; IQCJ-SCHIP1 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>PRDM1 (hacat_stim_2,hacat_stim only), TAD level:2; PREP (hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>PHRF1 (hacat_stim_2,hacat_stim only), TAD level:1; RASSF7 (hacat_stim_2,hacat_stim only), TAD level:1; DEAF1 (hacat_stim only), TAD level:2; TMEM80 (hacat_stim only), TAD level:2; EPS8L2 (hacat_stim only), TAD level:2; TALDO1 (hacat_stim only), TAD level:2; GATD1 (hacat_stim only), TAD level:2; SLC25A22 (hacat_stim only), TAD level:2; PIDD1 (hacat_stim_2,hacat_stim only), TAD level:2; RPLP2 (hacat_stim_2,hacat_stim only), TAD level:2; BET1L (hacat_stim only), TAD level:not found; RIC8A (hacat_stim only), TAD level:not found; IRF7 (hacat_stim_2,hacat_stim only), TAD level:1; LMNTD2 (hacat_stim_2,hacat_stim only), TAD level:1; PANO1 (hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>RAB2A (hacat_stim only), TAD level:3; CHD7 (hacat_stim_2,hacat_stim only), TAD level:2; ASPH (hacat_stim only), TAD level:outside tad</t>
+    <t>CD81 (hacat_stim only), TAD level:4; TSSC4 (hacat_stim_2, hacat_stim only), TAD level:4</t>
+  </si>
+  <si>
+    <t>TNPO3 (hacat_stim_2, hacat_stim only), TAD level:2; IRF5 (hacat_stim_2, hacat_stim only), TAD level:2; KCP (hacat_stim_2, hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>GADD45A (hacat_stim_2 only), TAD level:outside tad; SERBP1 (hacat_stim_2, hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>NDST1 (hacat_stim only), TAD level:1; TNIP1 (hacat_stim only), TAD level:2; SYNPO (hacat_stim_2, hacat_stim only), TAD level:1; ATOX1 (hacat_stim_2 only), TAD level:not found; GM2A (hacat_stim_2 only), TAD level:2</t>
+  </si>
+  <si>
+    <t>STAT1 (hacat_stim_2, hacat_stim only), TAD level:not found; MFSD6 (hacat_stim_2, hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>IFT80 (hacat_stim_2, hacat_stim only), TAD level:2; SMC4 (hacat_stim_2, hacat_stim only), TAD level:not found; IQCJ-SCHIP1 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>PRDM1 (hacat_stim_2, hacat_stim only), TAD level:2; PREP (hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>PHRF1 (hacat_stim_2, hacat_stim only), TAD level:1; RASSF7 (hacat_stim_2, hacat_stim only), TAD level:1; DEAF1 (hacat_stim only), TAD level:2; TMEM80 (hacat_stim only), TAD level:2; EPS8L2 (hacat_stim only), TAD level:2; TALDO1 (hacat_stim only), TAD level:2; GATD1 (hacat_stim only), TAD level:2; SLC25A22 (hacat_stim only), TAD level:2; PIDD1 (hacat_stim_2, hacat_stim only), TAD level:2; RPLP2 (hacat_stim_2, hacat_stim only), TAD level:2; BET1L (hacat_stim only), TAD level:not found; RIC8A (hacat_stim only), TAD level:not found; IRF7 (hacat_stim_2, hacat_stim only), TAD level:1; LMNTD2 (hacat_stim_2, hacat_stim only), TAD level:1; PANO1 (hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>RAB2A (hacat_stim only), TAD level:3; CHD7 (hacat_stim_2, hacat_stim only), TAD level:2; ASPH (hacat_stim only), TAD level:outside tad</t>
   </si>
   <si>
     <t>GSDMB (all), TAD level:1; PSMD3 (all), TAD level:not found; STARD3 (all), TAD level:1; GRB7 (all), TAD level:1; MIEN1 (all), TAD level:1; ORMDL3 (all), TAD level:1</t>
   </si>
   <si>
-    <t>ARHGAP31 (hacat_stim_2,hacat_stim only), TAD level:not found; TIMMDC1 (hacat_stim_2,hacat_stim only), TAD level:1; COX17 (hacat_stim_2,hacat_stim only), TAD level:1; POGLUT1 (all), TAD level:1; TMEM39A (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>LLGL2 (hacat_unstim only), TAD level:3; CDR2L (hacat_unstim only), TAD level:not found; MRPS7 (all), TAD level:not found; GGA3 (all), TAD level:not found; ARMC7 (all), TAD level:1; NUP85 (all), TAD level:1; MIF4GD (all), TAD level:not found; HID1 (all), TAD level:not found; ATP5PD (hacat_unstim_2,hacat_unstim only), TAD level:1; CASKIN2 (hacat_unstim only), TAD level:3; TMEM94 (hacat_unstim_2,hacat_unstim only), TAD level:3; GRB2 (hacat_unstim_2,hacat_unstim only), TAD level:not found; KCTD2 (all), TAD level:1; TSEN54 (hacat_unstim only), TAD level:3</t>
+    <t>ARHGAP31 (hacat_stim_2, hacat_stim only), TAD level:not found; TIMMDC1 (hacat_stim_2, hacat_stim only), TAD level:1; COX17 (hacat_stim_2, hacat_stim only), TAD level:1; POGLUT1 (all), TAD level:1; TMEM39A (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>LLGL2 (hacat_unstim only), TAD level:3; CDR2L (hacat_unstim only), TAD level:not found; MRPS7 (all), TAD level:not found; GGA3 (all), TAD level:not found; ARMC7 (all), TAD level:1; NUP85 (all), TAD level:1; MIF4GD (all), TAD level:not found; HID1 (all), TAD level:not found; ATP5PD (hacat_unstim_2, hacat_unstim only), TAD level:1; CASKIN2 (hacat_unstim only), TAD level:3; TMEM94 (hacat_unstim_2, hacat_unstim only), TAD level:3; GRB2 (hacat_unstim_2, hacat_unstim only), TAD level:not found; KCTD2 (all), TAD level:1; TSEN54 (hacat_unstim only), TAD level:3</t>
   </si>
   <si>
     <t>DDX6 (all), TAD level:2; UPK2 (hacat_unstim only), TAD level:2; CCDC84 (hacat_unstim only), TAD level:2; BCL9L (all), TAD level:2</t>
   </si>
   <si>
-    <t>TMEM175 (hacat_unstim_2,hacat_unstim only), TAD level:1; DGKQ (all), TAD level:not found; ATP5ME (hacat_unstim only), TAD level:outside tad; GAK (hacat_unstim_2,hacat_unstim only), TAD level:1; MYL5 (hacat_unstim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>IRF5 (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>CSK (all), TAD level:4; C15orf39 (hacat_unstim_2 only), TAD level:2; RPP25 (all), TAD level:4; COX5A (hacat_unstim_1,hacat_unstim only), TAD level:4; FAM219B (all), TAD level:4</t>
-  </si>
-  <si>
-    <t>NAB1 (all), TAD level:1; INPP1 (hacat_unstim_2,hacat_unstim only), TAD level:not found; MFSD6 (hacat_unstim_2,hacat_unstim only), TAD level:1; NEMP2 (all), TAD level:1; HIBCH (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>DARS2 (hacat_unstim_2,hacat_unstim only), TAD level:5; CENPL (hacat_unstim_2,hacat_unstim only), TAD level:5; RABGAP1L (hacat_unstim only), TAD level:not found</t>
+    <t>TMEM175 (hacat_unstim_2, hacat_unstim only), TAD level:1; DGKQ (all), TAD level:not found; ATP5ME (hacat_unstim only), TAD level:outside tad; GAK (hacat_unstim_2, hacat_unstim only), TAD level:1; MYL5 (hacat_unstim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>IRF5 (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>CSK (all), TAD level:4; C15orf39 (hacat_unstim_2 only), TAD level:2; RPP25 (all), TAD level:4; COX5A (hacat_unstim_1, hacat_unstim only), TAD level:4; FAM219B (all), TAD level:4</t>
+  </si>
+  <si>
+    <t>NAB1 (all), TAD level:1; INPP1 (hacat_unstim_2, hacat_unstim only), TAD level:not found; MFSD6 (hacat_unstim_2, hacat_unstim only), TAD level:1; NEMP2 (all), TAD level:1; HIBCH (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>DARS2 (hacat_unstim_2, hacat_unstim only), TAD level:5; CENPL (hacat_unstim_2, hacat_unstim only), TAD level:5; RABGAP1L (hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
     <t>ZBTB37 (hacat_unstim only), TAD level:5</t>
   </si>
   <si>
-    <t>POU2F1 (hacat_unstim_2,hacat_unstim only), TAD level:2; TADA1 (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>NFKB1 (all), TAD level:1; UBE2D3 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>CD81 (hacat_unstim only), TAD level:2; TSSC4 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>TNPO3 (all), TAD level:3; IRF5 (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
+    <t>POU2F1 (hacat_unstim_2, hacat_unstim only), TAD level:2; TADA1 (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>NFKB1 (all), TAD level:1; UBE2D3 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>CD81 (hacat_unstim only), TAD level:2; TSSC4 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>TNPO3 (all), TAD level:3; IRF5 (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
   </si>
   <si>
     <t>SERBP1 (hacat_unstim only), TAD level:1</t>
   </si>
   <si>
-    <t>MFSD6 (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
+    <t>MFSD6 (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
     <t>IFT80 (hacat_unstim only), TAD level:2; SMC4 (hacat_unstim only), TAD level:not found</t>
@@ -1259,55 +1259,55 @@
     <t>PRDM1 (hacat_unstim_2 only), TAD level:2</t>
   </si>
   <si>
-    <t>PHRF1 (hacat_unstim_2,hacat_unstim only), TAD level:1; RASSF7 (hacat_unstim_2,hacat_unstim only), TAD level:1; HRAS (hacat_unstim only), TAD level:2; DEAF1 (hacat_unstim_1,hacat_unstim only), TAD level:2; TMEM80 (hacat_unstim_1,hacat_unstim only), TAD level:2; EPS8L2 (hacat_unstim_1,hacat_unstim only), TAD level:2; TALDO1 (hacat_unstim_2,hacat_unstim only), TAD level:2; SLC25A22 (hacat_unstim only), TAD level:2; PIDD1 (hacat_unstim only), TAD level:not found; RPLP2 (hacat_unstim only), TAD level:not found; BET1L (hacat_unstim_2,hacat_unstim only), TAD level:not found; RIC8A (hacat_unstim_2,hacat_unstim only), TAD level:not found; IRF7 (hacat_unstim_2,hacat_unstim only), TAD level:1; LMNTD2 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>CHD7 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>PSMD3 (hacat_unstim_2,hacat_unstim only), TAD level:not found; STARD3 (hacat_unstim_2,hacat_unstim only), TAD level:1; GRB7 (hacat_unstim_2,hacat_unstim only), TAD level:1; MIEN1 (hacat_unstim_2,hacat_unstim only), TAD level:1; ORMDL3 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>ARHGAP31 (hacat_unstim_2,hacat_unstim only), TAD level:not found; TIMMDC1 (hacat_unstim_2,hacat_unstim only), TAD level:not found; COX17 (hacat_unstim_2,hacat_unstim only), TAD level:not found; POGLUT1 (all), TAD level:not found; TMEM39A (all), TAD level:not found</t>
-  </si>
-  <si>
-    <t>CDR2L (all), TAD level:not found; MRPS7 (all), TAD level:1; GGA3 (all), TAD level:1; ARMC7 (all), TAD level:2; NUP85 (all), TAD level:2; MIF4GD (all), TAD level:1; NT5C (myla_1,myla only), TAD level:2; GRB2 (all), TAD level:1; KCTD2 (myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>MCAM (myla_2,myla only), TAD level:3; DDX6 (all), TAD level:4</t>
-  </si>
-  <si>
-    <t>DGKQ (all), TAD level:2; GAK (myla only), TAD level:2; MYL5 (myla_2,myla only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>IRF5 (myla_1,myla only), TAD level:3</t>
-  </si>
-  <si>
-    <t>CSK (all), TAD level:5; ULK3 (all), TAD level:5; SCAMP2 (myla_1,myla only), TAD level:5; COX5A (all), TAD level:5; FAM219B (myla only), TAD level:5; CLK3 (all), TAD level:4</t>
-  </si>
-  <si>
-    <t>INPP1 (all), TAD level:2; MFSD6 (myla only), TAD level:4; NEMP2 (myla_1,myla only), TAD level:4; HIBCH (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>DARS2 (myla only), TAD level:5; CENPL (myla only), TAD level:5; RABGAP1L (myla_1,myla only), TAD level:3</t>
-  </si>
-  <si>
-    <t>UCK2 (myla only), TAD level:outside tad; TMCO1 (myla only), TAD level:outside tad; POU2F1 (myla_1,myla only), TAD level:1; MGST3 (myla only), TAD level:not found; TADA1 (myla_1,myla only), TAD level:not found; CD247 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>NFKB1 (all), TAD level:2; SLC9B2 (myla_1,myla only), TAD level:2; BDH2 (myla_1,myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>TNPO3 (all), TAD level:3; IRF5 (myla_1,myla only), TAD level:3; HILPDA (myla_1,myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>RBM22 (myla only), TAD level:2; G3BP1 (myla only), TAD level:not found; ATOX1 (myla_1,myla only), TAD level:not found; GM2A (myla only), TAD level:3</t>
+    <t>PHRF1 (hacat_unstim_2, hacat_unstim only), TAD level:1; RASSF7 (hacat_unstim_2, hacat_unstim only), TAD level:1; HRAS (hacat_unstim only), TAD level:2; DEAF1 (hacat_unstim_1, hacat_unstim only), TAD level:2; TMEM80 (hacat_unstim_1, hacat_unstim only), TAD level:2; EPS8L2 (hacat_unstim_1, hacat_unstim only), TAD level:2; TALDO1 (hacat_unstim_2, hacat_unstim only), TAD level:2; SLC25A22 (hacat_unstim only), TAD level:2; PIDD1 (hacat_unstim only), TAD level:not found; RPLP2 (hacat_unstim only), TAD level:not found; BET1L (hacat_unstim_2, hacat_unstim only), TAD level:not found; RIC8A (hacat_unstim_2, hacat_unstim only), TAD level:not found; IRF7 (hacat_unstim_2, hacat_unstim only), TAD level:1; LMNTD2 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>CHD7 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>PSMD3 (hacat_unstim_2, hacat_unstim only), TAD level:not found; STARD3 (hacat_unstim_2, hacat_unstim only), TAD level:1; GRB7 (hacat_unstim_2, hacat_unstim only), TAD level:1; MIEN1 (hacat_unstim_2, hacat_unstim only), TAD level:1; ORMDL3 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>ARHGAP31 (hacat_unstim_2, hacat_unstim only), TAD level:not found; TIMMDC1 (hacat_unstim_2, hacat_unstim only), TAD level:not found; COX17 (hacat_unstim_2, hacat_unstim only), TAD level:not found; POGLUT1 (all), TAD level:not found; TMEM39A (all), TAD level:not found</t>
+  </si>
+  <si>
+    <t>CDR2L (all), TAD level:not found; MRPS7 (all), TAD level:1; GGA3 (all), TAD level:1; ARMC7 (all), TAD level:2; NUP85 (all), TAD level:2; MIF4GD (all), TAD level:1; NT5C (myla_1, myla only), TAD level:2; GRB2 (all), TAD level:1; KCTD2 (myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>MCAM (myla_2, myla only), TAD level:3; DDX6 (all), TAD level:4</t>
+  </si>
+  <si>
+    <t>DGKQ (all), TAD level:2; GAK (myla only), TAD level:2; MYL5 (myla_2, myla only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>IRF5 (myla_1, myla only), TAD level:3</t>
+  </si>
+  <si>
+    <t>CSK (all), TAD level:5; ULK3 (all), TAD level:5; SCAMP2 (myla_1, myla only), TAD level:5; COX5A (all), TAD level:5; FAM219B (myla only), TAD level:5; CLK3 (all), TAD level:4</t>
+  </si>
+  <si>
+    <t>INPP1 (all), TAD level:2; MFSD6 (myla only), TAD level:4; NEMP2 (myla_1, myla only), TAD level:4; HIBCH (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>DARS2 (myla only), TAD level:5; CENPL (myla only), TAD level:5; RABGAP1L (myla_1, myla only), TAD level:3</t>
+  </si>
+  <si>
+    <t>UCK2 (myla only), TAD level:outside tad; TMCO1 (myla only), TAD level:outside tad; POU2F1 (myla_1, myla only), TAD level:1; MGST3 (myla only), TAD level:not found; TADA1 (myla_1, myla only), TAD level:not found; CD247 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>NFKB1 (all), TAD level:2; SLC9B2 (myla_1, myla only), TAD level:2; BDH2 (myla_1, myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>TNPO3 (all), TAD level:3; IRF5 (myla_1, myla only), TAD level:3; HILPDA (myla_1, myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>RBM22 (myla only), TAD level:2; G3BP1 (myla only), TAD level:not found; ATOX1 (myla_1, myla only), TAD level:not found; GM2A (myla only), TAD level:3</t>
   </si>
   <si>
     <t>MFSD6 (myla only), TAD level:not found</t>
   </si>
   <si>
-    <t>IFT80 (myla_1,myla only), TAD level:1; SMC4 (myla_1,myla only), TAD level:1; TRIM59 (myla_1,myla only), TAD level:not found</t>
+    <t>IFT80 (myla_1, myla only), TAD level:1; SMC4 (myla_1, myla only), TAD level:1; TRIM59 (myla_1, myla only), TAD level:not found</t>
   </si>
   <si>
     <t>PRDM1 (all), TAD level:1; PREP (myla only), TAD level:not found</t>
@@ -1322,16 +1322,16 @@
     <t>FLNB (myla_1 only), TAD level:3</t>
   </si>
   <si>
-    <t>CACNB1 (myla_1,myla only), TAD level:1; GSDMB (all), TAD level:2; RPL19 (myla_1,myla only), TAD level:1; PSMD3 (all), TAD level:not found; RPL23 (myla only), TAD level:1; STARD3 (all), TAD level:1; MIEN1 (myla only), TAD level:2; IKZF3 (all), TAD level:2; ORMDL3 (all), TAD level:2</t>
+    <t>CACNB1 (myla_1, myla only), TAD level:1; GSDMB (all), TAD level:2; RPL19 (myla_1, myla only), TAD level:1; PSMD3 (all), TAD level:not found; RPL23 (myla only), TAD level:1; STARD3 (all), TAD level:1; MIEN1 (myla only), TAD level:2; IKZF3 (all), TAD level:2; ORMDL3 (all), TAD level:2</t>
   </si>
   <si>
     <t>TIMMDC1 (myla_2 only), TAD level:1; COX17 (all), TAD level:1; PLA1A (myla only), TAD level:1; POGLUT1 (all), TAD level:1; TMEM39A (all), TAD level:1</t>
   </si>
   <si>
-    <t>LLGL2 (naive_T_2,naive_T only); MFSD11 (naive_T only); RECQL5 (all); MRPS7 (all); GGA3 (all); ARMC7 (all); NUP85 (all); SLC25A19 (naive_T only); MIF4GD (all); WBP2 (naive_T_1,naive_T only); H3F3B (all); UNK (all); TRIM65 (naive_T only); SAP30BP (all); SRSF2 (naive_T only); HID1 (naive_T_1,naive_T only); ATP5PD (all); TMEM94 (naive_T_1,naive_T only); GRB2 (all); KCTD2 (all); METTL23 (naive_T only); TSEN54 (naive_T_2,naive_T only); SUMO2 (naive_T_2 only); MRPL38 (naive_T only); MYO15B (naive_T only); AC005837.2 (naive_T only)</t>
-  </si>
-  <si>
-    <t>COX4I1 (naive_T_1,naive_T only); EMC8 (naive_T_1,naive_T only); IRF8 (naive_T_1,naive_T only)</t>
+    <t>LLGL2 (naive_T_2, naive_T only); MFSD11 (naive_T only); RECQL5 (all); MRPS7 (all); GGA3 (all); ARMC7 (all); NUP85 (all); SLC25A19 (naive_T only); MIF4GD (all); WBP2 (naive_T_1, naive_T only); H3F3B (all); UNK (all); TRIM65 (naive_T only); SAP30BP (all); SRSF2 (naive_T only); HID1 (naive_T_1, naive_T only); ATP5PD (all); TMEM94 (naive_T_1, naive_T only); GRB2 (all); KCTD2 (all); METTL23 (naive_T only); TSEN54 (naive_T_2, naive_T only); SUMO2 (naive_T_2 only); MRPL38 (naive_T only); MYO15B (naive_T only); AC005837.2 (naive_T only)</t>
+  </si>
+  <si>
+    <t>COX4I1 (naive_T_1, naive_T only); EMC8 (naive_T_1, naive_T only); IRF8 (naive_T_1, naive_T only)</t>
   </si>
   <si>
     <t>DDX6 (all); CXCR5 (all); CCDC84 (naive_T_1 only); BCL9L (all)</t>
@@ -1340,16 +1340,16 @@
     <t>IDUA (all); FGFRL1 (naive_T only); DGKQ (all); UVSSA (naive_T only)</t>
   </si>
   <si>
-    <t>CSK (all); C15orf39 (all); SIN3A (all); COX5A (all); CLK3 (naive_T_2,naive_T only)</t>
-  </si>
-  <si>
-    <t>STAT4 (all); NAB1 (all); INPP1 (naive_T only); MFSD6 (all); NABP1 (all); NEMP2 (all); HIBCH (naive_T_1,naive_T only)</t>
+    <t>CSK (all); C15orf39 (all); SIN3A (all); COX5A (all); CLK3 (naive_T_2, naive_T only)</t>
+  </si>
+  <si>
+    <t>STAT4 (all); NAB1 (all); INPP1 (naive_T only); MFSD6 (all); NABP1 (all); NEMP2 (all); HIBCH (naive_T_1, naive_T only)</t>
   </si>
   <si>
     <t>BLZF1 (naive_T_2 only); NME7 (naive_T_2 only); GPA33 (all); POU2F1 (all); TADA1 (all); CD247 (all)</t>
   </si>
   <si>
-    <t>NFKB1 (all); MANBA (naive_T_2,naive_T only); UBE2D3 (all); PPP3CA (naive_T only); SLC39A8 (all); CISD2 (all); SLC9B1 (all); SLC9B2 (naive_T_2,naive_T only); BDH2 (naive_T_2,naive_T only)</t>
+    <t>NFKB1 (all); MANBA (naive_T_2, naive_T only); UBE2D3 (all); PPP3CA (naive_T only); SLC39A8 (all); CISD2 (all); SLC9B1 (all); SLC9B2 (naive_T_2, naive_T only); BDH2 (naive_T_2, naive_T only)</t>
   </si>
   <si>
     <t>TSSC4 (naive_T only)</t>
@@ -1358,7 +1358,7 @@
     <t>TNPO3 (all); CALU (naive_T only); METTL2B (naive_T_2 only)</t>
   </si>
   <si>
-    <t>CD74 (all); DCTN4 (naive_T_1,naive_T only); RPS14 (all); GM2A (naive_T only)</t>
+    <t>CD74 (all); DCTN4 (naive_T_1, naive_T only); RPS14 (all); GM2A (naive_T only)</t>
   </si>
   <si>
     <t>STAT1 (naive_T_2 only); STAT4 (all); MFSD6 (all); NABP1 (all)</t>
@@ -1370,16 +1370,16 @@
     <t>PRDM1 (all)</t>
   </si>
   <si>
-    <t>PHRF1 (all); RASSF7 (all); SIRT3 (naive_T only); DEAF1 (all); TMEM80 (all); EPS8L2 (all); TALDO1 (naive_T_1,naive_T only); GATD1 (naive_T_1,naive_T only); SLC25A22 (all); PIDD1 (all); RPLP2 (naive_T_2,naive_T only); BET1L (naive_T_1,naive_T only); RIC8A (naive_T_1,naive_T only); IRF7 (all); LMNTD2 (all); PSMD13 (naive_T only); PANO1 (all)</t>
-  </si>
-  <si>
-    <t>NSMAF (naive_T only); CHD7 (all); ASPH (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>GSDMB (all); PSMD3 (naive_T_1,naive_T_2 only); STARD3 (all); MIEN1 (naive_T_2,naive_T only); IKZF3 (all); ORMDL3 (all); EIF1 (naive_T only); TCAP (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>NDUFB4 (all); GSK3B (all); TIMMDC1 (all); B4GALT4 (all); COX17 (all); RABL3 (all); GTF2E1 (all); POGLUT1 (all); LRRC58 (naive_T_2,naive_T only); TMEM39A (all)</t>
+    <t>PHRF1 (all); RASSF7 (all); SIRT3 (naive_T only); DEAF1 (all); TMEM80 (all); EPS8L2 (all); TALDO1 (naive_T_1, naive_T only); GATD1 (naive_T_1, naive_T only); SLC25A22 (all); PIDD1 (all); RPLP2 (naive_T_2, naive_T only); BET1L (naive_T_1, naive_T only); RIC8A (naive_T_1, naive_T only); IRF7 (all); LMNTD2 (all); PSMD13 (naive_T only); PANO1 (all)</t>
+  </si>
+  <si>
+    <t>NSMAF (naive_T only); CHD7 (all); ASPH (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>GSDMB (all); PSMD3 (naive_T_1, naive_T_2 only); STARD3 (all); MIEN1 (naive_T_2, naive_T only); IKZF3 (all); ORMDL3 (all); EIF1 (naive_T only); TCAP (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>NDUFB4 (all); GSK3B (all); TIMMDC1 (all); B4GALT4 (all); COX17 (all); RABL3 (all); GTF2E1 (all); POGLUT1 (all); LRRC58 (naive_T_2, naive_T only); TMEM39A (all)</t>
   </si>
   <si>
     <t>rs10794648</t>
@@ -1802,142 +1802,142 @@
     <t>STK24; GPR18; TM9SF2; UBAC2; GPR183</t>
   </si>
   <si>
-    <t>STPG1 (all), TAD level:4; NIPAL3 (all), TAD level:4; SRRM1 (hacat_stim_2,hacat_stim only), TAD level:2; IL22RA1 (hacat_stim_2 only), TAD level:3; GRHL3 (hacat_stim only), TAD level:4; CLIC4 (hacat_stim only), TAD level:1</t>
+    <t>STPG1 (all), TAD level:4; NIPAL3 (all), TAD level:4; SRRM1 (hacat_stim_2, hacat_stim only), TAD level:2; IL22RA1 (hacat_stim_2 only), TAD level:3; GRHL3 (hacat_stim only), TAD level:4; CLIC4 (hacat_stim only), TAD level:1</t>
   </si>
   <si>
     <t>CLEC2B (hacat_stim only), TAD level:1</t>
   </si>
   <si>
-    <t>RPL6 (hacat_stim_2,hacat_stim only), TAD level:1; MAPKAPK5 (hacat_stim_2,hacat_stim only), TAD level:not found; BRAP (hacat_stim_2 only), TAD level:1; ERP29 (hacat_stim_2,hacat_stim only), TAD level:1; ACAD10 (hacat_stim_2 only), TAD level:1; NAA25 (all), TAD level:1; TRAFD1 (hacat_stim_2,hacat_stim only), TAD level:1; HECTD4 (hacat_stim_2,hacat_stim only), TAD level:1; PTPN11 (hacat_stim_2,hacat_stim only), TAD level:not found; TMEM116 (hacat_stim_2,hacat_stim only), TAD level:1; ATXN2 (hacat_stim_2,hacat_stim only), TAD level:1</t>
+    <t>RPL6 (hacat_stim_2, hacat_stim only), TAD level:1; MAPKAPK5 (hacat_stim_2, hacat_stim only), TAD level:not found; BRAP (hacat_stim_2 only), TAD level:1; ERP29 (hacat_stim_2, hacat_stim only), TAD level:1; ACAD10 (hacat_stim_2 only), TAD level:1; NAA25 (all), TAD level:1; TRAFD1 (hacat_stim_2, hacat_stim only), TAD level:1; HECTD4 (hacat_stim_2, hacat_stim only), TAD level:1; PTPN11 (hacat_stim_2, hacat_stim only), TAD level:not found; TMEM116 (hacat_stim_2, hacat_stim only), TAD level:1; ATXN2 (hacat_stim_2, hacat_stim only), TAD level:1</t>
   </si>
   <si>
     <t>ZMIZ1 (all), TAD level:1; RPS24 (hacat_stim only), TAD level:not found; POLR3A (hacat_stim only), TAD level:outside tad</t>
   </si>
   <si>
-    <t>SERBP1 (hacat_stim_2,hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>DDX58 (hacat_stim_1,hacat_stim only), TAD level:2; APTX (hacat_stim only), TAD level:not found; TOPORS (all), TAD level:2; SMIM27 (all), TAD level:2</t>
+    <t>SERBP1 (hacat_stim_2, hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>DDX58 (hacat_stim_1, hacat_stim only), TAD level:2; APTX (hacat_stim only), TAD level:not found; TOPORS (all), TAD level:2; SMIM27 (all), TAD level:2</t>
   </si>
   <si>
     <t>SUCO (hacat_stim only), TAD level:4</t>
   </si>
   <si>
-    <t>KLF4 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>RAB27B (hacat_stim_2,hacat_stim only), TAD level:outside tad; POLI (all), TAD level:2; MBD2 (all), TAD level:1; C18orf54 (hacat_stim_2,hacat_stim only), TAD level:not found</t>
+    <t>KLF4 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>RAB27B (hacat_stim_2, hacat_stim only), TAD level:outside tad; POLI (all), TAD level:2; MBD2 (all), TAD level:1; C18orf54 (hacat_stim_2, hacat_stim only), TAD level:not found</t>
   </si>
   <si>
     <t>NFKBIZ (hacat_stim only), TAD level:2</t>
   </si>
   <si>
-    <t>RUNX1 (hacat_stim_2,hacat_stim only), TAD level:5; CBR1 (hacat_stim only), TAD level:5; SETD4 (hacat_stim only), TAD level:5</t>
-  </si>
-  <si>
-    <t>PPP2R3C (hacat_stim_2,hacat_stim only), TAD level:2; KIAA0391 (hacat_stim_2,hacat_stim only), TAD level:2; PSMA6 (hacat_stim_2,hacat_stim only), TAD level:3; NFKBIA (hacat_stim_2,hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>VCL (hacat_stim_2,hacat_stim only), TAD level:1; PLAU (hacat_stim_2,hacat_stim only), TAD level:2; ADK (hacat_stim only), TAD level:1; SAMD8 (hacat_stim_2,hacat_stim only), TAD level:1; VDAC2 (all), TAD level:1; COMTD1 (hacat_stim_2,hacat_stim only), TAD level:1; C10orf55 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>ERAP1 (hacat_stim_2,hacat_stim only), TAD level:2; ERAP2 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>KLF13 (hacat_stim_1,hacat_stim only), TAD level:4</t>
-  </si>
-  <si>
-    <t>AC118549.1 (hacat_stim_2,hacat_stim only), TAD level:not found; USP33 (hacat_stim only), TAD level:not found; GIPC2 (hacat_stim_2,hacat_stim only), TAD level:not found; FUBP1 (all), TAD level:not found; DNAJB4 (hacat_stim_2,hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>ICAM3 (hacat_stim only), TAD level:2; ICAM1 (all), TAD level:2; MRPL4 (all), TAD level:2; ICAM5 (all), TAD level:2; TYK2 (hacat_stim_2,hacat_stim only), TAD level:2; DNMT1 (hacat_stim_2,hacat_stim only), TAD level:1; RAVER1 (hacat_stim only), TAD level:2; ZGLP1 (hacat_stim_2,hacat_stim only), TAD level:2; FDX2 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>NEK7 (hacat_stim_2,hacat_stim only), TAD level:3; C1orf53 (hacat_stim_2,hacat_stim only), TAD level:4; DENND1B (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>PFKFB2 (hacat_stim_2 only), TAD level:not found; MAPKAPK2 (hacat_stim_2,hacat_stim only), TAD level:1; C1orf116 (hacat_stim_2 only), TAD level:1; RASSF5 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>CLEC16A (all), TAD level:not found; RMI2 (hacat_stim_2,hacat_stim only), TAD level:2; DEXI (all), TAD level:not found; SNN (hacat_stim_2,hacat_stim only), TAD level:2; SOCS1 (all), TAD level:3</t>
-  </si>
-  <si>
-    <t>FDX1 (hacat_stim_2,hacat_stim only), TAD level:not found; ZC3H12C (all), TAD level:1</t>
+    <t>RUNX1 (hacat_stim_2, hacat_stim only), TAD level:5; CBR1 (hacat_stim only), TAD level:5; SETD4 (hacat_stim only), TAD level:5</t>
+  </si>
+  <si>
+    <t>PPP2R3C (hacat_stim_2, hacat_stim only), TAD level:2; KIAA0391 (hacat_stim_2, hacat_stim only), TAD level:2; PSMA6 (hacat_stim_2, hacat_stim only), TAD level:3; NFKBIA (hacat_stim_2, hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>VCL (hacat_stim_2, hacat_stim only), TAD level:1; PLAU (hacat_stim_2, hacat_stim only), TAD level:2; ADK (hacat_stim only), TAD level:1; SAMD8 (hacat_stim_2, hacat_stim only), TAD level:1; VDAC2 (all), TAD level:1; COMTD1 (hacat_stim_2, hacat_stim only), TAD level:1; C10orf55 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>ERAP1 (hacat_stim_2, hacat_stim only), TAD level:2; ERAP2 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>KLF13 (hacat_stim_1, hacat_stim only), TAD level:4</t>
+  </si>
+  <si>
+    <t>AC118549.1 (hacat_stim_2, hacat_stim only), TAD level:not found; USP33 (hacat_stim only), TAD level:not found; GIPC2 (hacat_stim_2, hacat_stim only), TAD level:not found; FUBP1 (all), TAD level:not found; DNAJB4 (hacat_stim_2, hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>ICAM3 (hacat_stim only), TAD level:2; ICAM1 (all), TAD level:2; MRPL4 (all), TAD level:2; ICAM5 (all), TAD level:2; TYK2 (hacat_stim_2, hacat_stim only), TAD level:2; DNMT1 (hacat_stim_2, hacat_stim only), TAD level:1; RAVER1 (hacat_stim only), TAD level:2; ZGLP1 (hacat_stim_2, hacat_stim only), TAD level:2; FDX2 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>NEK7 (hacat_stim_2, hacat_stim only), TAD level:3; C1orf53 (hacat_stim_2, hacat_stim only), TAD level:4; DENND1B (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>PFKFB2 (hacat_stim_2 only), TAD level:not found; MAPKAPK2 (hacat_stim_2, hacat_stim only), TAD level:1; C1orf116 (hacat_stim_2 only), TAD level:1; RASSF5 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>CLEC16A (all), TAD level:not found; RMI2 (hacat_stim_2, hacat_stim only), TAD level:2; DEXI (all), TAD level:not found; SNN (hacat_stim_2, hacat_stim only), TAD level:2; SOCS1 (all), TAD level:3</t>
+  </si>
+  <si>
+    <t>FDX1 (hacat_stim_2, hacat_stim only), TAD level:not found; ZC3H12C (all), TAD level:1</t>
   </si>
   <si>
     <t>DNM2 (hacat_stim only), TAD level:1; QTRT1 (hacat_stim only), TAD level:1</t>
   </si>
   <si>
-    <t>CA11 (hacat_stim_2,hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>RECQL5 (hacat_stim only), TAD level:2; GALK1 (all), TAD level:4; WBP2 (all), TAD level:4; H3F3B (all), TAD level:4; UNK (all), TAD level:4; TRIM47 (all), TAD level:4; TRIM65 (hacat_stim_2,hacat_stim only), TAD level:3; SAP30BP (hacat_stim only), TAD level:2; ACOX1 (hacat_stim_2,hacat_stim only), TAD level:3; EVPL (hacat_stim_2,hacat_stim only), TAD level:4; SRP68 (hacat_stim_2,hacat_stim only), TAD level:4; EXOC7 (hacat_stim_2,hacat_stim only), TAD level:4; FBF1 (hacat_stim_2,hacat_stim only), TAD level:3</t>
+    <t>CA11 (hacat_stim_2, hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>RECQL5 (hacat_stim only), TAD level:2; GALK1 (all), TAD level:4; WBP2 (all), TAD level:4; H3F3B (all), TAD level:4; UNK (all), TAD level:4; TRIM47 (all), TAD level:4; TRIM65 (hacat_stim_2, hacat_stim only), TAD level:3; SAP30BP (hacat_stim only), TAD level:2; ACOX1 (hacat_stim_2, hacat_stim only), TAD level:3; EVPL (hacat_stim_2, hacat_stim only), TAD level:4; SRP68 (hacat_stim_2, hacat_stim only), TAD level:4; EXOC7 (hacat_stim_2, hacat_stim only), TAD level:4; FBF1 (hacat_stim_2, hacat_stim only), TAD level:3</t>
   </si>
   <si>
     <t>CEP76 (hacat_stim only), TAD level:1; PSMG2 (hacat_stim only), TAD level:1; PTPN2 (hacat_stim only), TAD level:2</t>
   </si>
   <si>
-    <t>ARVCF (hacat_stim only), TAD level:not found; MED15 (hacat_stim_2,hacat_stim only), TAD level:outside tad; CRKL (hacat_stim_2,hacat_stim only), TAD level:not found; LZTR1 (hacat_stim_2,hacat_stim only), TAD level:not found; SDF2L1 (hacat_stim_2,hacat_stim only), TAD level:1; YDJC (all), TAD level:1; TANGO2 (hacat_stim only), TAD level:outside tad; UBE2L3 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>PERP (hacat_stim_2,hacat_stim only), TAD level:outside tad; TNFAIP3 (hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>ZNFX1 (hacat_stim_2,hacat_stim only), TAD level:not found; RNF114 (all), TAD level:not found; TMEM189 (all), TAD level:2; UBE2V1 (hacat_stim_2,hacat_stim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>ABCC2 (all), TAD level:1; CWF19L1 (all), TAD level:2; DNMBP (hacat_stim_2,hacat_stim only), TAD level:1; ERLIN1 (hacat_stim_2,hacat_stim only), TAD level:2; ENTPD7 (hacat_stim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>PRSS8 (hacat_stim_2,hacat_stim only), TAD level:3; FUS (hacat_stim_2,hacat_stim only), TAD level:2; FBXL19 (all), TAD level:not found; HSD3B7 (all), TAD level:not found; SETD1A (all), TAD level:not found; ZNF629 (hacat_stim only), TAD level:5; PYCARD (all), TAD level:2; STX4 (all), TAD level:3; BCKDK (hacat_stim_2,hacat_stim only), TAD level:3; KAT8 (hacat_stim_2,hacat_stim only), TAD level:3; RNF40 (hacat_stim_2,hacat_stim only), TAD level:5; TGFB1I1 (hacat_stim only), TAD level:2; C16orf58 (hacat_stim only), TAD level:1; ARMC5 (all), TAD level:2; PRR14 (hacat_stim_2 only), TAD level:4; FBRS (hacat_stim_2 only), TAD level:4; PHKG2 (hacat_stim_2,hacat_stim only), TAD level:5; ZNF668 (all), TAD level:3; ZNF646 (all), TAD level:3; VKORC1 (hacat_stim_2,hacat_stim only), TAD level:3; ZNF267 (hacat_stim_2,hacat_stim only), TAD level:not found; CCDC189 (hacat_stim_2,hacat_stim only), TAD level:5</t>
-  </si>
-  <si>
-    <t>FOXO1 (hacat_stim_2,hacat_stim only), TAD level:4</t>
+    <t>ARVCF (hacat_stim only), TAD level:not found; MED15 (hacat_stim_2, hacat_stim only), TAD level:outside tad; CRKL (hacat_stim_2, hacat_stim only), TAD level:not found; LZTR1 (hacat_stim_2, hacat_stim only), TAD level:not found; SDF2L1 (hacat_stim_2, hacat_stim only), TAD level:1; YDJC (all), TAD level:1; TANGO2 (hacat_stim only), TAD level:outside tad; UBE2L3 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>PERP (hacat_stim_2, hacat_stim only), TAD level:outside tad; TNFAIP3 (hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>ZNFX1 (hacat_stim_2, hacat_stim only), TAD level:not found; RNF114 (all), TAD level:not found; TMEM189 (all), TAD level:2; UBE2V1 (hacat_stim_2, hacat_stim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>ABCC2 (all), TAD level:1; CWF19L1 (all), TAD level:2; DNMBP (hacat_stim_2, hacat_stim only), TAD level:1; ERLIN1 (hacat_stim_2, hacat_stim only), TAD level:2; ENTPD7 (hacat_stim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>PRSS8 (hacat_stim_2, hacat_stim only), TAD level:3; FUS (hacat_stim_2, hacat_stim only), TAD level:2; FBXL19 (all), TAD level:not found; HSD3B7 (all), TAD level:not found; SETD1A (all), TAD level:not found; ZNF629 (hacat_stim only), TAD level:5; PYCARD (all), TAD level:2; STX4 (all), TAD level:3; BCKDK (hacat_stim_2, hacat_stim only), TAD level:3; KAT8 (hacat_stim_2, hacat_stim only), TAD level:3; RNF40 (hacat_stim_2, hacat_stim only), TAD level:5; TGFB1I1 (hacat_stim only), TAD level:2; C16orf58 (hacat_stim only), TAD level:1; ARMC5 (all), TAD level:2; PRR14 (hacat_stim_2 only), TAD level:4; FBRS (hacat_stim_2 only), TAD level:4; PHKG2 (hacat_stim_2, hacat_stim only), TAD level:5; ZNF668 (all), TAD level:3; ZNF646 (all), TAD level:3; VKORC1 (hacat_stim_2, hacat_stim only), TAD level:3; ZNF267 (hacat_stim_2, hacat_stim only), TAD level:not found; CCDC189 (hacat_stim_2, hacat_stim only), TAD level:5</t>
+  </si>
+  <si>
+    <t>FOXO1 (hacat_stim_2, hacat_stim only), TAD level:4</t>
   </si>
   <si>
     <t>ERRFI1 (all), TAD level:not found</t>
   </si>
   <si>
-    <t>PTEN (hacat_stim_2,hacat_stim only), TAD level:3; KLLN (hacat_stim_2,hacat_stim only), TAD level:3</t>
-  </si>
-  <si>
-    <t>STAT3 (hacat_stim only), TAD level:3; CAVIN1 (hacat_stim_2,hacat_stim only), TAD level:4</t>
-  </si>
-  <si>
-    <t>BAD (all), TAD level:1; CAPN1 (hacat_stim_2,hacat_stim only), TAD level:1; PRDX5 (hacat_stim_2,hacat_stim only), TAD level:not found; WDR74 (hacat_stim_2,hacat_stim only), TAD level:outside tad; MTA2 (hacat_stim only), TAD level:outside tad; EML3 (hacat_stim only), TAD level:outside tad; RPS6KA4 (all), TAD level:not found; CDC42BPG (hacat_stim only), TAD level:1; TRMT112 (hacat_stim_2,hacat_stim only), TAD level:1; ESRRA (hacat_stim_2,hacat_stim only), TAD level:1; GPR137 (all), TAD level:1; PPP1R14B (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>REV3L (all), TAD level:1; TRAF3IP2 (hacat_stim_2,hacat_stim only), TAD level:3; MFSD4B (hacat_stim_2,hacat_stim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>DOCK9 (hacat_stim_2,hacat_stim only), TAD level:not found; TM9SF2 (hacat_stim_2,hacat_stim only), TAD level:2; UBAC2 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>STPG1 (all), TAD level:3; NIPAL3 (all), TAD level:3; SRRM1 (hacat_unstim_2,hacat_unstim only), TAD level:2; GRHL3 (all), TAD level:3</t>
+    <t>PTEN (hacat_stim_2, hacat_stim only), TAD level:3; KLLN (hacat_stim_2, hacat_stim only), TAD level:3</t>
+  </si>
+  <si>
+    <t>STAT3 (hacat_stim only), TAD level:3; CAVIN1 (hacat_stim_2, hacat_stim only), TAD level:4</t>
+  </si>
+  <si>
+    <t>BAD (all), TAD level:1; CAPN1 (hacat_stim_2, hacat_stim only), TAD level:1; PRDX5 (hacat_stim_2, hacat_stim only), TAD level:not found; WDR74 (hacat_stim_2, hacat_stim only), TAD level:outside tad; MTA2 (hacat_stim only), TAD level:outside tad; EML3 (hacat_stim only), TAD level:outside tad; RPS6KA4 (all), TAD level:not found; CDC42BPG (hacat_stim only), TAD level:1; TRMT112 (hacat_stim_2, hacat_stim only), TAD level:1; ESRRA (hacat_stim_2, hacat_stim only), TAD level:1; GPR137 (all), TAD level:1; PPP1R14B (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>REV3L (all), TAD level:1; TRAF3IP2 (hacat_stim_2, hacat_stim only), TAD level:3; MFSD4B (hacat_stim_2, hacat_stim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>DOCK9 (hacat_stim_2, hacat_stim only), TAD level:not found; TM9SF2 (hacat_stim_2, hacat_stim only), TAD level:2; UBAC2 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>STPG1 (all), TAD level:3; NIPAL3 (all), TAD level:3; SRRM1 (hacat_unstim_2, hacat_unstim only), TAD level:2; GRHL3 (all), TAD level:3</t>
   </si>
   <si>
     <t>YBX3 (hacat_unstim only), TAD level:not found; CLEC2B (hacat_unstim only), TAD level:1; TMEM52B (hacat_unstim only), TAD level:1; OLR1 (hacat_unstim only), TAD level:1</t>
   </si>
   <si>
-    <t>RPL6 (hacat_unstim_2,hacat_unstim only), TAD level:1; BRAP (hacat_unstim only), TAD level:1; ERP29 (hacat_unstim_2,hacat_unstim only), TAD level:1; ACAD10 (hacat_unstim only), TAD level:1; NAA25 (all), TAD level:1; TRAFD1 (hacat_unstim only), TAD level:1; HECTD4 (hacat_unstim only), TAD level:1; PTPN11 (hacat_unstim_2,hacat_unstim only), TAD level:not found; TMEM116 (hacat_unstim_2,hacat_unstim only), TAD level:1; ATXN2 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>ZMIZ1 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
+    <t>RPL6 (hacat_unstim_2, hacat_unstim only), TAD level:1; BRAP (hacat_unstim only), TAD level:1; ERP29 (hacat_unstim_2, hacat_unstim only), TAD level:1; ACAD10 (hacat_unstim only), TAD level:1; NAA25 (all), TAD level:1; TRAFD1 (hacat_unstim only), TAD level:1; HECTD4 (hacat_unstim only), TAD level:1; PTPN11 (hacat_unstim_2, hacat_unstim only), TAD level:not found; TMEM116 (hacat_unstim_2, hacat_unstim only), TAD level:1; ATXN2 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>ZMIZ1 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
   </si>
   <si>
     <t>SLC35D1 (hacat_unstim_2 only), TAD level:1; SERBP1 (hacat_unstim only), TAD level:1</t>
   </si>
   <si>
-    <t>ACO1 (hacat_unstim only), TAD level:not found; APTX (hacat_unstim only), TAD level:not found; NDUFB6 (hacat_unstim only), TAD level:1; TOPORS (hacat_unstim_2,hacat_unstim only), TAD level:1; SMIM27 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>SUCO (hacat_unstim_2,hacat_unstim only), TAD level:5</t>
+    <t>ACO1 (hacat_unstim only), TAD level:not found; APTX (hacat_unstim only), TAD level:not found; NDUFB6 (hacat_unstim only), TAD level:1; TOPORS (hacat_unstim_2, hacat_unstim only), TAD level:1; SMIM27 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>SUCO (hacat_unstim_2, hacat_unstim only), TAD level:5</t>
   </si>
   <si>
     <t>KLF4 (all), TAD level:2</t>
   </si>
   <si>
-    <t>RAB27B (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; POLI (all), TAD level:2; MBD2 (all), TAD level:1; C18orf54 (hacat_unstim only), TAD level:not found</t>
+    <t>RAB27B (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; POLI (all), TAD level:2; MBD2 (all), TAD level:1; C18orf54 (hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
     <t>PSMD14 (hacat_unstim only), TAD level:not found</t>
@@ -1946,61 +1946,61 @@
     <t>RUNX1 (all), TAD level:3</t>
   </si>
   <si>
-    <t>VCL (hacat_unstim_2,hacat_unstim only), TAD level:1; PLAU (hacat_unstim_2,hacat_unstim only), TAD level:2; SAMD8 (hacat_unstim only), TAD level:1; VDAC2 (all), TAD level:1; COMTD1 (hacat_unstim only), TAD level:1; C10orf55 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>ERAP1 (hacat_unstim_2,hacat_unstim only), TAD level:2; ERAP2 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
-  </si>
-  <si>
-    <t>FUBP1 (all), TAD level:not found; DNAJB4 (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>ICAM3 (hacat_unstim only), TAD level:1; ICAM5 (all), TAD level:1; TYK2 (hacat_unstim_2,hacat_unstim only), TAD level:1; DNMT1 (hacat_unstim only), TAD level:1; RAVER1 (hacat_unstim only), TAD level:1; FDX2 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
+    <t>VCL (hacat_unstim_2, hacat_unstim only), TAD level:1; PLAU (hacat_unstim_2, hacat_unstim only), TAD level:2; SAMD8 (hacat_unstim only), TAD level:1; VDAC2 (all), TAD level:1; COMTD1 (hacat_unstim only), TAD level:1; C10orf55 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>ERAP1 (hacat_unstim_2, hacat_unstim only), TAD level:2; ERAP2 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
+  </si>
+  <si>
+    <t>FUBP1 (all), TAD level:not found; DNAJB4 (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>ICAM3 (hacat_unstim only), TAD level:1; ICAM5 (all), TAD level:1; TYK2 (hacat_unstim_2, hacat_unstim only), TAD level:1; DNMT1 (hacat_unstim only), TAD level:1; RAVER1 (hacat_unstim only), TAD level:1; FDX2 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
   </si>
   <si>
     <t>PUS10 (hacat_unstim only), TAD level:2; PEX13 (hacat_unstim only), TAD level:1</t>
   </si>
   <si>
-    <t>C1orf53 (hacat_unstim_2,hacat_unstim only), TAD level:4; DENND1B (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>MAPKAPK2 (hacat_unstim_2,hacat_unstim only), TAD level:1; RASSF5 (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>CLEC16A (hacat_unstim_2,hacat_unstim only), TAD level:not found; DEXI (hacat_unstim_2,hacat_unstim only), TAD level:not found</t>
+    <t>C1orf53 (hacat_unstim_2, hacat_unstim only), TAD level:4; DENND1B (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>MAPKAPK2 (hacat_unstim_2, hacat_unstim only), TAD level:1; RASSF5 (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>CLEC16A (hacat_unstim_2, hacat_unstim only), TAD level:not found; DEXI (hacat_unstim_2, hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
     <t>ZC3H12C (all), TAD level:1; DDX10 (hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
-    <t>DNM2 (hacat_unstim_2,hacat_unstim only), TAD level:1; QTRT1 (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>CA11 (hacat_unstim_2,hacat_unstim only), TAD level:not found; DBP (hacat_unstim only), TAD level:not found</t>
+    <t>DNM2 (hacat_unstim_2, hacat_unstim only), TAD level:1; QTRT1 (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>CA11 (hacat_unstim_2, hacat_unstim only), TAD level:not found; DBP (hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
     <t>TSC22D1 (hacat_unstim_2 only), TAD level:2</t>
   </si>
   <si>
-    <t>RECQL5 (hacat_unstim only), TAD level:2; GALK1 (all), TAD level:3; WBP2 (all), TAD level:3; H3F3B (all), TAD level:3; UNK (all), TAD level:3; TRIM47 (all), TAD level:3; TRIM65 (hacat_unstim only), TAD level:1; SAP30BP (hacat_unstim only), TAD level:2; ACOX1 (hacat_unstim only), TAD level:1; EVPL (hacat_unstim only), TAD level:2; SRP68 (hacat_unstim_2,hacat_unstim only), TAD level:2; EXOC7 (hacat_unstim only), TAD level:2; GALR2 (hacat_unstim_2 only), TAD level:2; UBALD2 (hacat_unstim_2,hacat_unstim only), TAD level:2</t>
+    <t>RECQL5 (hacat_unstim only), TAD level:2; GALK1 (all), TAD level:3; WBP2 (all), TAD level:3; H3F3B (all), TAD level:3; UNK (all), TAD level:3; TRIM47 (all), TAD level:3; TRIM65 (hacat_unstim only), TAD level:1; SAP30BP (hacat_unstim only), TAD level:2; ACOX1 (hacat_unstim only), TAD level:1; EVPL (hacat_unstim only), TAD level:2; SRP68 (hacat_unstim_2, hacat_unstim only), TAD level:2; EXOC7 (hacat_unstim only), TAD level:2; GALR2 (hacat_unstim_2 only), TAD level:2; UBALD2 (hacat_unstim_2, hacat_unstim only), TAD level:2</t>
   </si>
   <si>
     <t>TRMT2A (hacat_unstim only), TAD level:outside tad; RANBP1 (hacat_unstim only), TAD level:outside tad; MED15 (hacat_unstim only), TAD level:outside tad; YDJC (all), TAD level:2; UBE2L3 (all), TAD level:2</t>
   </si>
   <si>
-    <t>PERP (hacat_unstim_1,hacat_unstim only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>RNF114 (all), TAD level:not found; TMEM189 (hacat_unstim_2,hacat_unstim only), TAD level:2; UBE2V1 (hacat_unstim_2 only), TAD level:2</t>
+    <t>PERP (hacat_unstim_1, hacat_unstim only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>RNF114 (all), TAD level:not found; TMEM189 (hacat_unstim_2, hacat_unstim only), TAD level:2; UBE2V1 (hacat_unstim_2 only), TAD level:2</t>
   </si>
   <si>
     <t>COX15 (hacat_unstim only), TAD level:not found; ABCC2 (all), TAD level:not found; CWF19L1 (all), TAD level:1; DNMBP (hacat_unstim_2 only), TAD level:1; CUTC (hacat_unstim only), TAD level:not found</t>
   </si>
   <si>
-    <t>ETS1 (all), TAD level:2; TMEM45B (hacat_unstim_2,hacat_unstim only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>PRSS8 (all), TAD level:4; FUS (hacat_unstim_2 only), TAD level:3; FBXL19 (all), TAD level:not found; HSD3B7 (all), TAD level:not found; SETD1A (all), TAD level:not found; ZNF629 (hacat_unstim_2,hacat_unstim only), TAD level:4; STX4 (all), TAD level:4; RNF40 (hacat_unstim_2,hacat_unstim only), TAD level:4; TGFB1I1 (hacat_unstim_2,hacat_unstim only), TAD level:2; ARMC5 (all), TAD level:2; PHKG2 (hacat_unstim_2,hacat_unstim only), TAD level:4; ZNF668 (all), TAD level:4; ZNF646 (all), TAD level:4; VKORC1 (all), TAD level:4; ZNF267 (hacat_unstim_1,hacat_unstim only), TAD level:2; CCDC189 (hacat_unstim_2,hacat_unstim only), TAD level:4</t>
+    <t>ETS1 (all), TAD level:2; TMEM45B (hacat_unstim_2, hacat_unstim only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>PRSS8 (all), TAD level:4; FUS (hacat_unstim_2 only), TAD level:3; FBXL19 (all), TAD level:not found; HSD3B7 (all), TAD level:not found; SETD1A (all), TAD level:not found; ZNF629 (hacat_unstim_2, hacat_unstim only), TAD level:4; STX4 (all), TAD level:4; RNF40 (hacat_unstim_2, hacat_unstim only), TAD level:4; TGFB1I1 (hacat_unstim_2, hacat_unstim only), TAD level:2; ARMC5 (all), TAD level:2; PHKG2 (hacat_unstim_2, hacat_unstim only), TAD level:4; ZNF668 (all), TAD level:4; ZNF646 (all), TAD level:4; VKORC1 (all), TAD level:4; ZNF267 (hacat_unstim_1, hacat_unstim only), TAD level:2; CCDC189 (hacat_unstim_2, hacat_unstim only), TAD level:4</t>
   </si>
   <si>
     <t>FOXO1 (all), TAD level:4</t>
@@ -2009,43 +2009,43 @@
     <t>ERRFI1 (all), TAD level:2</t>
   </si>
   <si>
-    <t>PTEN (hacat_unstim_2,hacat_unstim only), TAD level:3; KLLN (hacat_unstim_2,hacat_unstim only), TAD level:3</t>
+    <t>PTEN (hacat_unstim_2, hacat_unstim only), TAD level:3; KLLN (hacat_unstim_2, hacat_unstim only), TAD level:3</t>
   </si>
   <si>
     <t>SOX4 (hacat_unstim only), TAD level:2</t>
   </si>
   <si>
-    <t>BAD (all), TAD level:1; CAPN1 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; MARK2 (hacat_unstim_2 only), TAD level:1; PRDX5 (all), TAD level:1; WDR74 (hacat_unstim_2,hacat_unstim only), TAD level:outside tad; MTA2 (hacat_unstim only), TAD level:outside tad; EML3 (hacat_unstim only), TAD level:outside tad; TTC9C (hacat_unstim only), TAD level:outside tad; RPS6KA4 (all), TAD level:not found; CDC42BPG (hacat_unstim only), TAD level:outside tad; TRMT112 (all), TAD level:1; ESRRA (all), TAD level:1; GPR137 (all), TAD level:1; PPP1R14B (all), TAD level:1; HNRNPUL2 (hacat_unstim only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>REV3L (hacat_unstim_2,hacat_unstim only), TAD level:1; MFSD4B (hacat_unstim_2,hacat_unstim only), TAD level:1</t>
-  </si>
-  <si>
-    <t>DOCK9 (hacat_unstim_2,hacat_unstim only), TAD level:not found; STK24 (hacat_unstim only), TAD level:outside tad; TM9SF2 (hacat_unstim_2,hacat_unstim only), TAD level:2; UBAC2 (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>RPL6 (all), TAD level:2; MAPKAPK5 (myla_1 only), TAD level:1; BRAP (myla only), TAD level:2; ERP29 (myla_1 only), TAD level:2; SH2B3 (all), TAD level:2; ACAD10 (myla only), TAD level:2; NAA25 (myla_1,myla only), TAD level:2; HECTD4 (all), TAD level:2; PTPN11 (all), TAD level:not found; TMEM116 (myla_1,myla only), TAD level:2; PHETA1 (myla only), TAD level:not found; ATXN2 (myla_1,myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>ZMIZ1 (all), TAD level:not found; RPS24 (myla_1,myla only), TAD level:1; POLR3A (myla_1,myla only), TAD level:1</t>
+    <t>BAD (all), TAD level:1; CAPN1 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; MARK2 (hacat_unstim_2 only), TAD level:1; PRDX5 (all), TAD level:1; WDR74 (hacat_unstim_2, hacat_unstim only), TAD level:outside tad; MTA2 (hacat_unstim only), TAD level:outside tad; EML3 (hacat_unstim only), TAD level:outside tad; TTC9C (hacat_unstim only), TAD level:outside tad; RPS6KA4 (all), TAD level:not found; CDC42BPG (hacat_unstim only), TAD level:outside tad; TRMT112 (all), TAD level:1; ESRRA (all), TAD level:1; GPR137 (all), TAD level:1; PPP1R14B (all), TAD level:1; HNRNPUL2 (hacat_unstim only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>REV3L (hacat_unstim_2, hacat_unstim only), TAD level:1; MFSD4B (hacat_unstim_2, hacat_unstim only), TAD level:1</t>
+  </si>
+  <si>
+    <t>DOCK9 (hacat_unstim_2, hacat_unstim only), TAD level:not found; STK24 (hacat_unstim only), TAD level:outside tad; TM9SF2 (hacat_unstim_2, hacat_unstim only), TAD level:2; UBAC2 (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>RPL6 (all), TAD level:2; MAPKAPK5 (myla_1 only), TAD level:1; BRAP (myla only), TAD level:2; ERP29 (myla_1 only), TAD level:2; SH2B3 (all), TAD level:2; ACAD10 (myla only), TAD level:2; NAA25 (myla_1, myla only), TAD level:2; HECTD4 (all), TAD level:2; PTPN11 (all), TAD level:not found; TMEM116 (myla_1, myla only), TAD level:2; PHETA1 (myla only), TAD level:not found; ATXN2 (myla_1, myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>ZMIZ1 (all), TAD level:not found; RPS24 (myla_1, myla only), TAD level:1; POLR3A (myla_1, myla only), TAD level:1</t>
   </si>
   <si>
     <t>ANLN (myla only), TAD level:not found; ELMO1 (all), TAD level:1; KIAA0895 (myla only), TAD level:not found</t>
   </si>
   <si>
-    <t>RAD50 (myla_1,myla only), TAD level:1; IL5 (all), TAD level:1; KIF3A (myla_1,myla only), TAD level:2</t>
+    <t>RAD50 (myla_1, myla only), TAD level:1; IL5 (all), TAD level:1; KIF3A (myla_1, myla only), TAD level:2</t>
   </si>
   <si>
     <t>BCL11B (myla_1 only), TAD level:2</t>
   </si>
   <si>
-    <t>POLI (all), TAD level:1; MBD2 (all), TAD level:not found; C18orf54 (myla only), TAD level:not found; TCF4 (myla_1,myla only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>NFKBIZ (myla_1,myla only), TAD level:not found; ZPLD1 (myla_1,myla_2 only), TAD level:not found</t>
-  </si>
-  <si>
-    <t>TANK (myla_1,myla only), TAD level:outside tad</t>
+    <t>POLI (all), TAD level:1; MBD2 (all), TAD level:not found; C18orf54 (myla only), TAD level:not found; TCF4 (myla_1, myla only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>NFKBIZ (myla_1, myla only), TAD level:not found; ZPLD1 (myla_1, myla_2 only), TAD level:not found</t>
+  </si>
+  <si>
+    <t>TANK (myla_1, myla only), TAD level:outside tad</t>
   </si>
   <si>
     <t>PPP2R3C (myla only), TAD level:2; KIAA0391 (myla only), TAD level:2</t>
@@ -2054,16 +2054,16 @@
     <t>RSPH3 (all), TAD level:2; TAGAP (all), TAD level:2</t>
   </si>
   <si>
-    <t>ADK (myla_1,myla only), TAD level:1; SAMD8 (myla_1,myla only), TAD level:1</t>
+    <t>ADK (myla_1, myla only), TAD level:1; SAMD8 (myla_1, myla only), TAD level:1</t>
   </si>
   <si>
     <t>GLRX (myla only), TAD level:outside tad; RGMB (myla only), TAD level:outside tad</t>
   </si>
   <si>
-    <t>AC118549.1 (myla_1,myla only), TAD level:4; FUBP1 (all), TAD level:4; DNAJB4 (myla_2,myla only), TAD level:4</t>
-  </si>
-  <si>
-    <t>ICAM3 (myla_1,myla only), TAD level:1; ICAM1 (all), TAD level:1; MRPL4 (myla_2 only), TAD level:1; ICAM5 (all), TAD level:1; TYK2 (all), TAD level:not found; ZGLP1 (myla only), TAD level:1; FDX2 (myla only), TAD level:1</t>
+    <t>AC118549.1 (myla_1, myla only), TAD level:4; FUBP1 (all), TAD level:4; DNAJB4 (myla_2, myla only), TAD level:4</t>
+  </si>
+  <si>
+    <t>ICAM3 (myla_1, myla only), TAD level:1; ICAM1 (all), TAD level:1; MRPL4 (myla_2 only), TAD level:1; ICAM5 (all), TAD level:1; TYK2 (all), TAD level:not found; ZGLP1 (myla only), TAD level:1; FDX2 (myla only), TAD level:1</t>
   </si>
   <si>
     <t>DENND1B (all), TAD level:not found</t>
@@ -2072,22 +2072,22 @@
     <t>RMI2 (all), TAD level:1; SOCS1 (all), TAD level:2</t>
   </si>
   <si>
-    <t>ZC3H12C (all), TAD level:3; NPAT (myla only), TAD level:2; ATM (myla only), TAD level:2; DDX10 (myla only), TAD level:2; LAYN (myla_1,myla only), TAD level:outside tad</t>
-  </si>
-  <si>
-    <t>UNC13D (myla_1 only), TAD level:not found; GALK1 (myla only), TAD level:not found; WBP2 (all), TAD level:2; H3F3B (myla_1,myla only), TAD level:not found; UNK (myla_1,myla only), TAD level:not found; TRIM47 (all), TAD level:2; ACOX1 (all), TAD level:2; EXOC7 (myla only), TAD level:2</t>
-  </si>
-  <si>
-    <t>PTPN2 (myla_1,myla only), TAD level:3</t>
-  </si>
-  <si>
-    <t>LZTR1 (myla_1,myla only), TAD level:outside tad; PPM1F (myla only), TAD level:outside tad; SDF2L1 (myla_2,myla only), TAD level:not found; YDJC (all), TAD level:not found; UBE2L3 (all), TAD level:not found</t>
+    <t>ZC3H12C (all), TAD level:3; NPAT (myla only), TAD level:2; ATM (myla only), TAD level:2; DDX10 (myla only), TAD level:2; LAYN (myla_1, myla only), TAD level:outside tad</t>
+  </si>
+  <si>
+    <t>UNC13D (myla_1 only), TAD level:not found; GALK1 (myla only), TAD level:not found; WBP2 (all), TAD level:2; H3F3B (myla_1, myla only), TAD level:not found; UNK (myla_1, myla only), TAD level:not found; TRIM47 (all), TAD level:2; ACOX1 (all), TAD level:2; EXOC7 (myla only), TAD level:2</t>
+  </si>
+  <si>
+    <t>PTPN2 (myla_1, myla only), TAD level:3</t>
+  </si>
+  <si>
+    <t>LZTR1 (myla_1, myla only), TAD level:outside tad; PPM1F (myla only), TAD level:outside tad; SDF2L1 (myla_2, myla only), TAD level:not found; YDJC (all), TAD level:not found; UBE2L3 (all), TAD level:not found</t>
   </si>
   <si>
     <t>TNFAIP3 (all), TAD level:5</t>
   </si>
   <si>
-    <t>RNF114 (all), TAD level:2; B4GALT5 (myla only), TAD level:3; SPATA2 (myla_1,myla only), TAD level:3; TMEM189 (myla_1,myla only), TAD level:4; UBE2V1 (myla only), TAD level:4</t>
+    <t>RNF114 (all), TAD level:2; B4GALT5 (myla only), TAD level:3; SPATA2 (myla_1, myla only), TAD level:3; TMEM189 (myla_1, myla only), TAD level:4; UBE2V1 (myla only), TAD level:4</t>
   </si>
   <si>
     <t>CWF19L1 (all), TAD level:1; ERLIN1 (myla only), TAD level:2; CHUK (myla only), TAD level:2</t>
@@ -2105,13 +2105,13 @@
     <t>KCNH4 (myla only), TAD level:2; STAT3 (all), TAD level:3</t>
   </si>
   <si>
-    <t>BAD (all), TAD level:2; FERMT3 (myla_1,myla only), TAD level:2; RPS6KA4 (myla only), TAD level:not found; CCDC88B (all), TAD level:not found; STIP1 (myla_1,myla only), TAD level:2; ESRRA (all), TAD level:2; GPR137 (all), TAD level:2; PPP1R14B (all), TAD level:2</t>
-  </si>
-  <si>
-    <t>DUSP22 (myla_1,myla only), TAD level:1; IRF4 (all), TAD level:1</t>
-  </si>
-  <si>
-    <t>STK24 (all), TAD level:1; GPR18 (myla_1,myla only), TAD level:1; TM9SF2 (myla_1,myla only), TAD level:not found; UBAC2 (all), TAD level:not found; GPR183 (myla_1,myla only), TAD level:1</t>
+    <t>BAD (all), TAD level:2; FERMT3 (myla_1, myla only), TAD level:2; RPS6KA4 (myla only), TAD level:not found; CCDC88B (all), TAD level:not found; STIP1 (myla_1, myla only), TAD level:2; ESRRA (all), TAD level:2; GPR137 (all), TAD level:2; PPP1R14B (all), TAD level:2</t>
+  </si>
+  <si>
+    <t>DUSP22 (myla_1, myla only), TAD level:1; IRF4 (all), TAD level:1</t>
+  </si>
+  <si>
+    <t>STK24 (all), TAD level:1; GPR18 (myla_1, myla only), TAD level:1; TM9SF2 (myla_1, myla only), TAD level:not found; UBAC2 (all), TAD level:not found; GPR183 (myla_1, myla only), TAD level:1</t>
   </si>
   <si>
     <t>STPG1 (all); NIPAL3 (naive_T only); SRRM1 (all)</t>
@@ -2120,7 +2120,7 @@
     <t>GABARAPL1 (naive_T only)</t>
   </si>
   <si>
-    <t>ANKRD13A (all); RPL6 (all); MAPKAPK5 (naive_T_1,naive_T only); BRAP (naive_T_2,naive_T only); ERP29 (naive_T_2,naive_T only); MVK (all); ARPC3 (naive_T_2 only); GPN3 (all); VPS29 (naive_T_2,naive_T only); SH2B3 (all); ACAD10 (naive_T_2,naive_T only); NAA25 (all); IFT81 (naive_T_2,naive_T only); TRAFD1 (naive_T_1,naive_T only); MMAB (all); GLTP (naive_T only); GIT2 (all); HECTD4 (all); C12orf76 (naive_T_1,naive_T only); PTPN11 (all); PPP1CC (all); ANAPC7 (all); PPTC7 (all); TMEM116 (naive_T_2,naive_T only); ATXN2 (all); TCTN1 (naive_T_1,naive_T only); FAM216A (all)</t>
+    <t>ANKRD13A (all); RPL6 (all); MAPKAPK5 (naive_T_1, naive_T only); BRAP (naive_T_2, naive_T only); ERP29 (naive_T_2, naive_T only); MVK (all); ARPC3 (naive_T_2 only); GPN3 (all); VPS29 (naive_T_2, naive_T only); SH2B3 (all); ACAD10 (naive_T_2, naive_T only); NAA25 (all); IFT81 (naive_T_2, naive_T only); TRAFD1 (naive_T_1, naive_T only); MMAB (all); GLTP (naive_T only); GIT2 (all); HECTD4 (all); C12orf76 (naive_T_1, naive_T only); PTPN11 (all); PPP1CC (all); ANAPC7 (all); PPTC7 (all); TMEM116 (naive_T_2, naive_T only); ATXN2 (all); TCTN1 (naive_T_1, naive_T only); FAM216A (all)</t>
   </si>
   <si>
     <t>ZMIZ1 (all)</t>
@@ -2132,10 +2132,10 @@
     <t>DNAJA1 (naive_T only); ACO1 (all); APTX (all); NDUFB6 (all); TOPORS (all); SMIM27 (all)</t>
   </si>
   <si>
-    <t>KAT5 (naive_T only); BANF1 (all); EIF1AD (all); SART1 (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>SUCO (naive_T_1,naive_T only); ZBTB37 (naive_T only)</t>
+    <t>KAT5 (naive_T only); BANF1 (all); EIF1AD (all); SART1 (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>SUCO (naive_T_1, naive_T only); ZBTB37 (naive_T only)</t>
   </si>
   <si>
     <t>PLCL2 (all)</t>
@@ -2150,67 +2150,67 @@
     <t>NFKBIZ (all)</t>
   </si>
   <si>
-    <t>PSMD14 (naive_T_2,naive_T only); GCA (naive_T_1 only)</t>
+    <t>PSMD14 (naive_T_2, naive_T only); GCA (naive_T_1 only)</t>
   </si>
   <si>
     <t>RUNX1 (all)</t>
   </si>
   <si>
-    <t>SERAC1 (naive_T_1,naive_T only); DYNLT1 (naive_T_1,naive_T only); SYTL3 (all); TAGAP (all); GTF2H5 (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>VCL (all); CAMK2G (all); ADK (naive_T_1,naive_T only); SAMD8 (all); VDAC2 (all); COMTD1 (all); AP3M1 (naive_T_1,naive_T only)</t>
+    <t>SERAC1 (naive_T_1, naive_T only); DYNLT1 (naive_T_1, naive_T only); SYTL3 (all); TAGAP (all); GTF2H5 (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>VCL (all); CAMK2G (all); ADK (naive_T_1, naive_T only); SAMD8 (all); VDAC2 (all); COMTD1 (all); AP3M1 (naive_T_1, naive_T only)</t>
   </si>
   <si>
     <t>RIOK2 (naive_T_2 only)</t>
   </si>
   <si>
-    <t>KLF13 (all); AC091057.6 (naive_T_2,naive_T only); ARHGAP11B (naive_T_2,naive_T only)</t>
-  </si>
-  <si>
-    <t>AC118549.1 (all); USP33 (all); IFI44L (naive_T only); IFI44 (naive_T_1,naive_T only); PIGK (naive_T_2 only); FUBP1 (all); DNAJB4 (all); MIGA1 (all)</t>
-  </si>
-  <si>
-    <t>ICAM3 (naive_T only); ICAM1 (all); MRPL4 (naive_T_2 only); TYK2 (all); PPAN (naive_T_1,naive_T only); ANGPTL6 (naive_T_1,naive_T only); RAVER1 (naive_T only); PPAN-P2RY11 (naive_T_1,naive_T only)</t>
+    <t>KLF13 (all); AC091057.6 (naive_T_2, naive_T only); ARHGAP11B (naive_T_2, naive_T only)</t>
+  </si>
+  <si>
+    <t>AC118549.1 (all); USP33 (all); IFI44L (naive_T only); IFI44 (naive_T_1, naive_T only); PIGK (naive_T_2 only); FUBP1 (all); DNAJB4 (all); MIGA1 (all)</t>
+  </si>
+  <si>
+    <t>ICAM3 (naive_T only); ICAM1 (all); MRPL4 (naive_T_2 only); TYK2 (all); PPAN (naive_T_1, naive_T only); ANGPTL6 (naive_T_1, naive_T only); RAVER1 (naive_T only); PPAN-P2RY11 (naive_T_1, naive_T only)</t>
   </si>
   <si>
     <t>ZBTB41 (naive_T only); DENND1B (all)</t>
   </si>
   <si>
-    <t>RASSF5 (naive_T_2,naive_T only)</t>
-  </si>
-  <si>
-    <t>CLEC16A (all); GSPT1 (all); ZC3H7A (all); TXNDC11 (all); RSL1D1 (naive_T only); RMI2 (naive_T_1,naive_T only); DEXI (all); SOCS1 (all)</t>
-  </si>
-  <si>
-    <t>DNM2 (all); ZNF791 (naive_T_2,naive_T only); ZNF490 (naive_T_2,naive_T only); QTRT1 (all)</t>
-  </si>
-  <si>
-    <t>CA11 (all); TBC1D17 (naive_T_1,naive_T only); CCDC114 (naive_T_2 only); RRAS (naive_T_1 only); SCAF1 (naive_T_1 only); EMP3 (naive_T_2 only); AKT1S1 (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>JMJD6 (naive_T_2,naive_T only); MFSD11 (naive_T only); GALK1 (naive_T only); MRPS7 (naive_T_1,naive_T only); GGA3 (naive_T_1,naive_T only); WBP2 (all); H3F3B (naive_T_1,naive_T only); UNK (naive_T_1,naive_T only); TRIM47 (all); TRIM65 (naive_T_2,naive_T only); ACOX1 (naive_T_2 only); PRPSAP1 (all); SRSF2 (naive_T only); KCTD2 (naive_T only); METTL23 (naive_T_2,naive_T only); TEN1 (naive_T_2 only); AC005837.2 (naive_T_2,naive_T only)</t>
+    <t>RASSF5 (naive_T_2, naive_T only)</t>
+  </si>
+  <si>
+    <t>CLEC16A (all); GSPT1 (all); ZC3H7A (all); TXNDC11 (all); RSL1D1 (naive_T only); RMI2 (naive_T_1, naive_T only); DEXI (all); SOCS1 (all)</t>
+  </si>
+  <si>
+    <t>DNM2 (all); ZNF791 (naive_T_2, naive_T only); ZNF490 (naive_T_2, naive_T only); QTRT1 (all)</t>
+  </si>
+  <si>
+    <t>CA11 (all); TBC1D17 (naive_T_1, naive_T only); CCDC114 (naive_T_2 only); RRAS (naive_T_1 only); SCAF1 (naive_T_1 only); EMP3 (naive_T_2 only); AKT1S1 (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>JMJD6 (naive_T_2, naive_T only); MFSD11 (naive_T only); GALK1 (naive_T only); MRPS7 (naive_T_1, naive_T only); GGA3 (naive_T_1, naive_T only); WBP2 (all); H3F3B (naive_T_1, naive_T only); UNK (naive_T_1, naive_T only); TRIM47 (all); TRIM65 (naive_T_2, naive_T only); ACOX1 (naive_T_2 only); PRPSAP1 (all); SRSF2 (naive_T only); KCTD2 (naive_T only); METTL23 (naive_T_2, naive_T only); TEN1 (naive_T_2 only); AC005837.2 (naive_T_2, naive_T only)</t>
   </si>
   <si>
     <t>SDF2L1 (all); YDJC (all); UBE2L3 (all)</t>
   </si>
   <si>
-    <t>CCDC28A (naive_T_1,naive_T only); IFNGR1 (all); BCLAF1 (all); PEX7 (naive_T only); HECA (naive_T_2,naive_T only); CITED2 (all); MAP3K5 (naive_T_1 only); GVQW2 (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>DPM1 (naive_T only); ZNFX1 (naive_T_1,naive_T only); CSE1L (naive_T_2 only); MOCS3 (naive_T only); RNF114 (all); DDX27 (naive_T_1,naive_T only); SPATA2 (naive_T_2 only); PTPN1 (naive_T_1,naive_T only); SLC9A8 (naive_T_1,naive_T only); UBE2V1 (naive_T_1,naive_T only)</t>
+    <t>CCDC28A (naive_T_1, naive_T only); IFNGR1 (all); BCLAF1 (all); PEX7 (naive_T only); HECA (naive_T_2, naive_T only); CITED2 (all); MAP3K5 (naive_T_1 only); GVQW2 (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>DPM1 (naive_T only); ZNFX1 (naive_T_1, naive_T only); CSE1L (naive_T_2 only); MOCS3 (naive_T only); RNF114 (all); DDX27 (naive_T_1, naive_T only); SPATA2 (naive_T_2 only); PTPN1 (naive_T_1, naive_T only); SLC9A8 (naive_T_1, naive_T only); UBE2V1 (naive_T_1, naive_T only)</t>
   </si>
   <si>
     <t>CWF19L1 (all); ERLIN1 (naive_T_2 only); CHUK (naive_T_2 only)</t>
   </si>
   <si>
-    <t>ETS1 (all); TMEM45B (naive_T_2,naive_T only); PRDM10 (naive_T_2,naive_T only)</t>
+    <t>ETS1 (all); TMEM45B (naive_T_2, naive_T only); PRDM10 (naive_T_2, naive_T only)</t>
   </si>
   <si>
     <t>RUNX3 (all)</t>
   </si>
   <si>
-    <t>SRCAP (all); FUS (all); FBXL19 (all); STX1B (all); SETD1A (all); BCL7C (naive_T only); PYCARD (naive_T only); STX4 (all); BCKDK (all); KAT8 (all); RNF40 (naive_T_2 only); SLC5A2 (all); C16orf58 (naive_T_1,naive_T only); ARMC5 (all); PRSS53 (all); ZNF668 (all); ZNF646 (all); VKORC1 (all); ZNF267 (all); CCDC189 (naive_T_2 only); ZNF720 (naive_T_2,naive_T only); AC135050.2 (all)</t>
+    <t>SRCAP (all); FUS (all); FBXL19 (all); STX1B (all); SETD1A (all); BCL7C (naive_T only); PYCARD (naive_T only); STX4 (all); BCKDK (all); KAT8 (all); RNF40 (naive_T_2 only); SLC5A2 (all); C16orf58 (naive_T_1, naive_T only); ARMC5 (all); PRSS53 (all); ZNF668 (all); ZNF646 (all); VKORC1 (all); ZNF267 (all); CCDC189 (naive_T_2 only); ZNF720 (naive_T_2, naive_T only); AC135050.2 (all)</t>
   </si>
   <si>
     <t>TBC1D5 (naive_T only); PLCL2 (all); SATB1 (all)</t>
@@ -2219,13 +2219,13 @@
     <t>PTEN (all); RNLS (naive_T_2 only)</t>
   </si>
   <si>
-    <t>BAD (all); PRDX5 (naive_T_2,naive_T only); WDR74 (all); FERMT3 (all); CCDC88B (all); STIP1 (all); TRMT112 (naive_T_2,naive_T only); ESRRA (all); GPR137 (all); PPP1R14B (all)</t>
-  </si>
-  <si>
-    <t>TUBE1 (naive_T only); MFSD4B (naive_T only); RPF2 (naive_T_1,naive_T only)</t>
-  </si>
-  <si>
-    <t>DOCK9 (naive_T_1,naive_T only); STK24 (naive_T_2,naive_T only); GPR18 (all); CLYBL (naive_T_2 only); TM9SF2 (all); GGACT (naive_T_2,naive_T only); UBAC2 (all)</t>
+    <t>BAD (all); PRDX5 (naive_T_2, naive_T only); WDR74 (all); FERMT3 (all); CCDC88B (all); STIP1 (all); TRMT112 (naive_T_2, naive_T only); ESRRA (all); GPR137 (all); PPP1R14B (all)</t>
+  </si>
+  <si>
+    <t>TUBE1 (naive_T only); MFSD4B (naive_T only); RPF2 (naive_T_1, naive_T only)</t>
+  </si>
+  <si>
+    <t>DOCK9 (naive_T_1, naive_T only); STK24 (naive_T_2, naive_T only); GPR18 (all); CLYBL (naive_T_2 only); TM9SF2 (all); GGACT (naive_T_2, naive_T only); UBAC2 (all)</t>
   </si>
 </sst>
 </file>

</xml_diff>